<commit_message>
1. Finalise performance template w/ IS-ENES3 submission example
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Example" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="&lt;Machine name&gt; performance for &lt;model name&gt;" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="HadGEM3-GC3.1 N512 ORCA12 on ARCHER-XC30" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="&lt;model name&gt; on &lt;machine name&gt;" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="84">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machine Performance</t>
   </si>
@@ -42,7 +42,7 @@
     <t xml:space="preserve">Machine</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;The machine this spreadsheet covers will be processed into this cell.&gt;</t>
+    <t xml:space="preserve">&lt;The machine that this spreadsheet concerns will be processed into this cell.&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">How to use</t>
@@ -51,25 +51,7 @@
     <t xml:space="preserve">https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Important</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: … [notes]</t>
-    </r>
+    <t xml:space="preserve">Note: each tab should record the representative performance of a single model on the given machine, where all applicable models were inferred from your machines spreadsheet submission. If any of the models registered for this machine are incorrect or missing (see the individual tabs) please contact the ES-DOC team via support@es-doc.org.</t>
   </si>
   <si>
     <t xml:space="preserve">Initialised by</t>
@@ -78,47 +60,13 @@
     <t xml:space="preserve">Internal notes</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;machine name&gt; performance for model &lt;model name&gt; in CMIP6</t>
+    <t xml:space="preserve">Performance of ARCHER-XC30 for model HadGEM3-GC3.1 N512 ORCA12</t>
   </si>
   <si>
     <t xml:space="preserve">Describes the properties of a performance of a configured model on a particular system/machine. Based on "CPMIP: Measurements of Real Computational Performance of Earth System Models" (Balaji et. al. 2016, doi:10.5194/gmd-2016-197).</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOTE: for further information about each metric to document, please refer to the corresponding metric covered in section 3 of the CPMIP defining paper linked above, though note also that it should not be necessary to consult the paper at all because </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">relevant parts of each description are provided here</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
+    <t xml:space="preserve">NOTE: for further information about each metric to document, please refer to the corresponding metric covered in section 3 of the CPMIP defining paper linked above, though note also that it should not be necessary to consult the paper at all because relevant parts of each description are provided here.</t>
   </si>
   <si>
     <t xml:space="preserve">Identity</t>
@@ -139,19 +87,22 @@
     <t xml:space="preserve">Name for performance (experiment/test/whatever).</t>
   </si>
   <si>
+    <t xml:space="preserve">ARCHER-XC30 representative performance for model HadGEM3-GC3.1 N512 ORCA12 in CMIP6</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Subcomponent performance</t>
   </si>
   <si>
-    <t xml:space="preserve">If machine is partitioned, treat subpartitions as machines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE 1: if the machine is not a partition of another machine, leave this field empty.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE 2: String must correspond to the name of another documented machine, i.e. a machine detailed in another tab. If the machine is not a partition, leave this field empty.</t>
+    <t xml:space="preserve">Describes the performance of each subcomponent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE 1: if the performance does not have subcomponents, please leave this field empty. If there is more than one subcomponent to cite, copy the row with the input cell and paste it below as many times as is necessary to fill out.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE 2: Each string must correspond to the name of another documented performance, i.e. a performance detailed in another tab.</t>
   </si>
   <si>
     <t xml:space="preserve">CPMIP Metrics: Model and Platform</t>
@@ -169,156 +120,172 @@
     <t xml:space="preserve">Platform on which performance was tested.</t>
   </si>
   <si>
+    <t xml:space="preserve">ARCHER-XC30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.2 *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model for which performance was tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HadGEM3-GC3.1 N512 ORCA12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution measured as the number of gridpoints (or more generally, spatial degrees of freedom) NX x NY x NZ per component with an independent discretization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complexity measured as the number of prognostic variables per component with an independent discretization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compiler used for performance test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCE 8.5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPMIP Metrics: Computational Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The computational cost metrics of CPMIP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated years per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated years per day (SYPD) in a 24h period on the given platform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual simulated years per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual simulated years per day (ASYPD) in a 24h period on the given platform obtained from a typical long-running simulation with the model. Inclusive of system interruptions, queue wait time, or issues with the model workflow, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core hours per simulated year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core-hours per simulated year (CHSY). This is measured as the product of the model runtime for 1 SY, and the numbers of cores allocated. Note that if allocations are done on a node basis then all cores on a node are charged against the allocation, regardless of whether or not they are used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joules per simulated year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The energy cost of a simulation, measured in joules per simulated year (JPSY). Given the energy E in joules consumed over a budgeting interval T (generally 1 month or 1 year, in units of hours), JPSY=CHSY*E*T/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallelisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or or all cores were used all of the time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further detail: CPMIP Metrics: Coupling, memory and I/O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information about how the various components of performance were related; set of additional information related to coupling, memory and I/O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling cost measures the overhead caused by coupling. This can include the cost of the coupling algorithm itself (which may involve grid interpolation and computation of transfer coefficients for conservative coupling) as well as load imbalance. It is the normalized difference between the time-processor integral for the whole model versus the sum of individual concurrent components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory bloat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size to the ideal memory size (the size of the complete model state, which in theory is all you need to hold in memory)Mi, defined below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data output cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data output cost is the cost of performing I/O, and is the ratio of CHSY with and without I/O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data intensity the amount of data produced per compute-hour, in units GB per compute-hour.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance of &lt;machine name&gt; for model &lt;model name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;machine name&gt; representative performance for model &lt;model name&gt; in CMIP6</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;name of machine in question (per spreadsheet) to be processed here&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.2 *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model for which performance was tested.</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;name of model in question (per tab) to be processed into here&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTEGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution measured as the number of gridpoints (or more generally, spatial degrees of freedom) NX x NY x NZ per component with an independent discretization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complexity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complexity measured as the number of prognostic variables per component with an independent discretization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compiler used for performance test.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPMIP Metrics: Computational Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The computational cost metrics of CPMIP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulated years per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLOAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulated years per day (SYPD) in a 24h period on the given platform.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual simulated years per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual simulated years per day (ASYPD) in a 24h period on the given platform obtained from a typical long-running simulation with the model. Inclusive of system interruptions, queue wait time, or issues with the model workflow, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core hours per simulated year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core-hours per simulated year (CHSY). This is measured as the product of the model runtime for 1 SY, and the numbers of cores allocated. Note that if allocations are done on a node basis then all cores on a node are charged against the allocation, regardless of whether or not they are used.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joules per simulated year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The energy cost of a simulation, measured in joules per simulated year (JPSY). Given the energy E in joules consumed over a budgeting interval T (generally 1 month or 1 year, in units of hours), JPSY=CHSY*E*T/NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallelisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or or all cores were used all of the time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further detail: CPMIP Metrics: Coupling, memory and I/O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information about how the various components of performance were related; set of additional information related to coupling, memory and I/O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupling cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupling cost measures the overhead caused by coupling. This can include the cost of the coupling algorithm itself (which may involve grid interpolation and computation of transfer coefficients for conservative coupling) as well as load imbalance. It is the normalized difference between the time-processor integral for the whole model versus the sum of individual concurrent components.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory bloat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size to the ideal memory size (the size of the complete model state, which in theory is all you need to hold in memory)Mi, defined below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data output cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data output cost is the cost of performing I/O, and is the ratio of CHSY with and without I/O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data intensity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data intensity the amount of data produced per compute-hour, in units GB per compute-hour.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -374,16 +341,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <b val="true"/>
       <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <u val="single"/>
       <sz val="18"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
@@ -396,14 +363,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -577,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -626,7 +585,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,15 +601,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,15 +621,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -674,43 +641,51 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,7 +769,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,6 +877,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/"/>
+    <hyperlink ref="B8" r:id="rId2" display="Note: each tab should record the representative performance of a single model on the given machine, where all applicable models were inferred from your machines spreadsheet submission. If any of the models registered for this machine are incorrect or missing (see the individual tabs) please contact the ES-DOC team via support@es-doc.org."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -920,8 +896,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -945,18 +921,18 @@
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" customFormat="false" ht="73.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" customFormat="false" ht="77.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -964,17 +940,17 @@
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="0"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="40.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="n">
@@ -986,17 +962,17 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -1004,41 +980,41 @@
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
-      <c r="B10" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="12"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -1046,67 +1022,67 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="26"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="26"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
-      <c r="B15" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="0"/>
+      <c r="B15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="0"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
-      <c r="B16" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="0"/>
-      <c r="F16" s="26"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="26"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -1114,71 +1090,71 @@
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="n">
         <v>1.2</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="19" t="s">
-        <v>27</v>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="0"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="0"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="26"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="24"/>
+      <c r="B23" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="25"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="26"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="B24" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="0"/>
-      <c r="F24" s="26"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
@@ -1186,79 +1162,79 @@
       <c r="C25" s="0"/>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="0"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="24"/>
+      <c r="B27" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="25"/>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
-      <c r="F27" s="26"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="B28" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="0"/>
-      <c r="F28" s="26"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="0"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="0"/>
-      <c r="F29" s="26"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="26"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="B31" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="26"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
     </row>
@@ -1271,34 +1247,34 @@
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
+      <c r="B34" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="24"/>
+      <c r="A35" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
     </row>
@@ -1311,14 +1287,14 @@
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
+      <c r="B38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
@@ -1326,19 +1302,21 @@
       <c r="A39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="24"/>
+      <c r="B39" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="25"/>
       <c r="D39" s="0"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
@@ -1355,7 +1333,7 @@
         <v>1.3</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -1364,51 +1342,53 @@
     </row>
     <row r="43" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="19" t="s">
-        <v>47</v>
+      <c r="B43" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C43" s="0"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
+      <c r="A45" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="24"/>
+      <c r="A46" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="25"/>
       <c r="D46" s="0"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
+      <c r="B47" s="26" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
@@ -1421,34 +1401,36 @@
       <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="A49" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
+      <c r="A50" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
+      <c r="B51" s="32" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
@@ -1461,34 +1443,36 @@
       <c r="F52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="A53" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
+      <c r="A54" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
+      <c r="B55" s="32" t="n">
+        <v>585540</v>
+      </c>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
@@ -1501,34 +1485,36 @@
       <c r="F56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
+      <c r="A57" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
+      <c r="A58" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
+      <c r="B59" s="34" t="n">
+        <v>23000000000</v>
+      </c>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
@@ -1541,34 +1527,36 @@
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
+      <c r="A61" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="24"/>
+      <c r="A62" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="25"/>
       <c r="D62" s="0"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
+      <c r="B63" s="26" t="n">
+        <v>12024</v>
+      </c>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
     </row>
@@ -1585,62 +1573,62 @@
         <v>1.4</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="26"/>
+      <c r="F65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="27"/>
-      <c r="B66" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
+      <c r="B66" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="26"/>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="23"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="0"/>
       <c r="E67" s="0"/>
-      <c r="F67" s="26"/>
+      <c r="F67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
+      <c r="A68" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="26"/>
+      <c r="F68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
+      <c r="A69" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="26"/>
+      <c r="F69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="26"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
@@ -1648,39 +1636,41 @@
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
       <c r="E71" s="0"/>
-      <c r="F71" s="26"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
+      <c r="A72" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="26"/>
+      <c r="F72" s="12"/>
     </row>
     <row r="73" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
+      <c r="A73" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="26"/>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
+      <c r="B74" s="26" t="n">
+        <v>183</v>
+      </c>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
       <c r="E74" s="0"/>
-      <c r="F74" s="26"/>
+      <c r="F74" s="12"/>
     </row>
     <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
@@ -1688,39 +1678,39 @@
       <c r="C75" s="0"/>
       <c r="D75" s="0"/>
       <c r="E75" s="0"/>
-      <c r="F75" s="26"/>
+      <c r="F75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
+      <c r="A76" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
       <c r="E76" s="0"/>
-      <c r="F76" s="26"/>
+      <c r="F76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="24"/>
+      <c r="A77" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="25"/>
       <c r="D77" s="0"/>
       <c r="E77" s="0"/>
-      <c r="F77" s="26"/>
+      <c r="F77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
       <c r="E78" s="0"/>
-      <c r="F78" s="26"/>
+      <c r="F78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
@@ -1728,39 +1718,41 @@
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
       <c r="E79" s="0"/>
-      <c r="F79" s="26"/>
+      <c r="F79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
+      <c r="A80" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="0"/>
-      <c r="F80" s="26"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="24"/>
+      <c r="A81" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="25"/>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
-      <c r="F81" s="26"/>
+      <c r="F81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
+      <c r="B82" s="26" t="n">
+        <v>207</v>
+      </c>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
       <c r="E82" s="0"/>
-      <c r="F82" s="26"/>
+      <c r="F82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
@@ -1768,15 +1760,15 @@
       <c r="C83" s="0"/>
       <c r="D83" s="0"/>
       <c r="E83" s="0"/>
-      <c r="F83" s="26"/>
+      <c r="F83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
-      <c r="B84" s="0"/>
-      <c r="C84" s="0"/>
-      <c r="D84" s="0"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="0"/>
-      <c r="F84" s="26"/>
+      <c r="F84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0"/>
@@ -1784,15 +1776,15 @@
       <c r="C85" s="0"/>
       <c r="D85" s="0"/>
       <c r="E85" s="0"/>
-      <c r="F85" s="26"/>
+      <c r="F85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
-      <c r="B86" s="0"/>
-      <c r="C86" s="0"/>
-      <c r="D86" s="0"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
       <c r="E86" s="0"/>
-      <c r="F86" s="26"/>
+      <c r="F86" s="12"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
@@ -1800,15 +1792,15 @@
       <c r="C87" s="0"/>
       <c r="D87" s="0"/>
       <c r="E87" s="0"/>
-      <c r="F87" s="26"/>
+      <c r="F87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
-      <c r="B88" s="0"/>
-      <c r="C88" s="0"/>
-      <c r="D88" s="0"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
       <c r="E88" s="0"/>
-      <c r="F88" s="26"/>
+      <c r="F88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0"/>
@@ -1816,15 +1808,15 @@
       <c r="C89" s="0"/>
       <c r="D89" s="0"/>
       <c r="E89" s="0"/>
-      <c r="F89" s="26"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
-      <c r="B90" s="0"/>
-      <c r="C90" s="0"/>
-      <c r="D90" s="0"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
       <c r="E90" s="0"/>
-      <c r="F90" s="26"/>
+      <c r="F90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
@@ -1832,15 +1824,15 @@
       <c r="C91" s="0"/>
       <c r="D91" s="0"/>
       <c r="E91" s="0"/>
-      <c r="F91" s="26"/>
+      <c r="F91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0"/>
-      <c r="B92" s="0"/>
-      <c r="C92" s="0"/>
-      <c r="D92" s="0"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
       <c r="E92" s="0"/>
-      <c r="F92" s="26"/>
+      <c r="F92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
@@ -1848,15 +1840,15 @@
       <c r="C93" s="0"/>
       <c r="D93" s="0"/>
       <c r="E93" s="0"/>
-      <c r="F93" s="26"/>
+      <c r="F93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
-      <c r="B94" s="0"/>
-      <c r="C94" s="0"/>
-      <c r="D94" s="0"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="0"/>
-      <c r="F94" s="26"/>
+      <c r="F94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
@@ -1864,15 +1856,15 @@
       <c r="C95" s="0"/>
       <c r="D95" s="0"/>
       <c r="E95" s="0"/>
-      <c r="F95" s="26"/>
+      <c r="F95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
-      <c r="B96" s="0"/>
-      <c r="C96" s="0"/>
-      <c r="D96" s="0"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
       <c r="E96" s="0"/>
-      <c r="F96" s="26"/>
+      <c r="F96" s="12"/>
     </row>
     <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
@@ -1880,15 +1872,15 @@
       <c r="C97" s="0"/>
       <c r="D97" s="0"/>
       <c r="E97" s="0"/>
-      <c r="F97" s="26"/>
+      <c r="F97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
-      <c r="B98" s="0"/>
-      <c r="C98" s="0"/>
-      <c r="D98" s="0"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
       <c r="E98" s="0"/>
-      <c r="F98" s="26"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
@@ -1896,15 +1888,15 @@
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
       <c r="E99" s="0"/>
-      <c r="F99" s="26"/>
+      <c r="F99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
-      <c r="B100" s="0"/>
-      <c r="C100" s="0"/>
-      <c r="D100" s="0"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
       <c r="E100" s="0"/>
-      <c r="F100" s="26"/>
+      <c r="F100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
@@ -1912,15 +1904,15 @@
       <c r="C101" s="0"/>
       <c r="D101" s="0"/>
       <c r="E101" s="0"/>
-      <c r="F101" s="26"/>
+      <c r="F101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
-      <c r="B102" s="0"/>
-      <c r="C102" s="0"/>
-      <c r="D102" s="0"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
       <c r="E102" s="0"/>
-      <c r="F102" s="26"/>
+      <c r="F102" s="12"/>
     </row>
     <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
@@ -1928,15 +1920,15 @@
       <c r="C103" s="0"/>
       <c r="D103" s="0"/>
       <c r="E103" s="0"/>
-      <c r="F103" s="26"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
-      <c r="B104" s="0"/>
-      <c r="C104" s="0"/>
-      <c r="D104" s="0"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
       <c r="E104" s="0"/>
-      <c r="F104" s="26"/>
+      <c r="F104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0"/>
@@ -1944,15 +1936,15 @@
       <c r="C105" s="0"/>
       <c r="D105" s="0"/>
       <c r="E105" s="0"/>
-      <c r="F105" s="26"/>
+      <c r="F105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0"/>
-      <c r="B106" s="0"/>
-      <c r="C106" s="0"/>
-      <c r="D106" s="0"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
       <c r="E106" s="0"/>
-      <c r="F106" s="26"/>
+      <c r="F106" s="12"/>
     </row>
     <row r="107" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0"/>
@@ -1960,15 +1952,15 @@
       <c r="C107" s="0"/>
       <c r="D107" s="0"/>
       <c r="E107" s="0"/>
-      <c r="F107" s="26"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0"/>
-      <c r="B108" s="0"/>
-      <c r="C108" s="0"/>
-      <c r="D108" s="0"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
       <c r="E108" s="0"/>
-      <c r="F108" s="26"/>
+      <c r="F108" s="12"/>
     </row>
     <row r="109" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0"/>
@@ -1976,15 +1968,15 @@
       <c r="C109" s="0"/>
       <c r="D109" s="0"/>
       <c r="E109" s="0"/>
-      <c r="F109" s="26"/>
+      <c r="F109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0"/>
-      <c r="B110" s="0"/>
-      <c r="C110" s="0"/>
-      <c r="D110" s="0"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
       <c r="E110" s="0"/>
-      <c r="F110" s="26"/>
+      <c r="F110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0"/>
@@ -1992,15 +1984,15 @@
       <c r="C111" s="0"/>
       <c r="D111" s="0"/>
       <c r="E111" s="0"/>
-      <c r="F111" s="26"/>
+      <c r="F111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0"/>
-      <c r="B112" s="0"/>
-      <c r="C112" s="0"/>
-      <c r="D112" s="0"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
       <c r="E112" s="0"/>
-      <c r="F112" s="26"/>
+      <c r="F112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0"/>
@@ -2008,206 +2000,206 @@
       <c r="C113" s="0"/>
       <c r="D113" s="0"/>
       <c r="E113" s="0"/>
-      <c r="F113" s="26"/>
+      <c r="F113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
-      <c r="B114" s="0"/>
-      <c r="C114" s="0"/>
-      <c r="D114" s="0"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
       <c r="E114" s="0"/>
-      <c r="F114" s="26"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
       <c r="B115" s="0"/>
       <c r="C115" s="0"/>
       <c r="D115" s="0"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="26"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0"/>
-      <c r="B116" s="0"/>
-      <c r="C116" s="0"/>
-      <c r="D116" s="0"/>
-      <c r="F116" s="26"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="33"/>
-      <c r="B117" s="33"/>
-      <c r="C117" s="33"/>
-      <c r="D117" s="33"/>
+      <c r="A117" s="36"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="36"/>
+      <c r="D117" s="36"/>
       <c r="E117" s="0"/>
-      <c r="F117" s="26"/>
+      <c r="F117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="33"/>
-      <c r="B118" s="33"/>
-      <c r="C118" s="33"/>
-      <c r="D118" s="33"/>
+      <c r="A118" s="36"/>
+      <c r="B118" s="36"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
       <c r="E118" s="0"/>
-      <c r="F118" s="26"/>
+      <c r="F118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="33"/>
-      <c r="B119" s="33"/>
-      <c r="C119" s="33"/>
-      <c r="D119" s="33"/>
+      <c r="A119" s="36"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="37"/>
       <c r="E119" s="0"/>
-      <c r="F119" s="26"/>
+      <c r="F119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="33"/>
-      <c r="B120" s="33"/>
-      <c r="C120" s="33"/>
-      <c r="D120" s="33"/>
+      <c r="A120" s="36"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="36"/>
+      <c r="D120" s="36"/>
       <c r="E120" s="0"/>
-      <c r="F120" s="26"/>
+      <c r="F120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="33"/>
-      <c r="B121" s="33"/>
-      <c r="C121" s="33"/>
-      <c r="D121" s="33"/>
+      <c r="A121" s="36"/>
+      <c r="B121" s="37"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="37"/>
       <c r="E121" s="0"/>
-      <c r="F121" s="26"/>
+      <c r="F121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="33"/>
-      <c r="B122" s="33"/>
-      <c r="C122" s="33"/>
-      <c r="D122" s="33"/>
+      <c r="A122" s="36"/>
+      <c r="B122" s="36"/>
+      <c r="C122" s="36"/>
+      <c r="D122" s="36"/>
       <c r="E122" s="0"/>
-      <c r="F122" s="26"/>
+      <c r="F122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="33"/>
-      <c r="B123" s="33"/>
-      <c r="C123" s="33"/>
-      <c r="D123" s="33"/>
+      <c r="A123" s="36"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="36"/>
+      <c r="D123" s="36"/>
       <c r="E123" s="0"/>
-      <c r="F123" s="26"/>
+      <c r="F123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="33"/>
-      <c r="B124" s="33"/>
-      <c r="C124" s="33"/>
-      <c r="D124" s="33"/>
+      <c r="A124" s="36"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="37"/>
+      <c r="D124" s="37"/>
       <c r="E124" s="0"/>
-      <c r="F124" s="26"/>
+      <c r="F124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="33"/>
-      <c r="B125" s="33"/>
-      <c r="C125" s="33"/>
-      <c r="D125" s="33"/>
+      <c r="A125" s="36"/>
+      <c r="B125" s="36"/>
+      <c r="C125" s="36"/>
+      <c r="D125" s="36"/>
       <c r="E125" s="0"/>
-      <c r="F125" s="26"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="33"/>
-      <c r="B126" s="33"/>
-      <c r="C126" s="33"/>
-      <c r="D126" s="33"/>
+      <c r="A126" s="36"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="37"/>
+      <c r="D126" s="37"/>
       <c r="E126" s="0"/>
-      <c r="F126" s="26"/>
+      <c r="F126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="33"/>
-      <c r="B127" s="33"/>
-      <c r="C127" s="33"/>
-      <c r="D127" s="33"/>
+      <c r="A127" s="36"/>
+      <c r="B127" s="36"/>
+      <c r="C127" s="36"/>
+      <c r="D127" s="36"/>
       <c r="E127" s="0"/>
-      <c r="F127" s="26"/>
+      <c r="F127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="33"/>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33"/>
-      <c r="D128" s="33"/>
+      <c r="A128" s="36"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
       <c r="E128" s="0"/>
-      <c r="F128" s="26"/>
+      <c r="F128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="33"/>
-      <c r="B129" s="33"/>
-      <c r="C129" s="33"/>
-      <c r="D129" s="33"/>
+      <c r="A129" s="36"/>
+      <c r="B129" s="36"/>
+      <c r="C129" s="36"/>
+      <c r="D129" s="36"/>
       <c r="E129" s="0"/>
-      <c r="F129" s="26"/>
+      <c r="F129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="33"/>
-      <c r="B130" s="33"/>
-      <c r="C130" s="33"/>
-      <c r="D130" s="33"/>
+      <c r="A130" s="36"/>
+      <c r="B130" s="36"/>
+      <c r="C130" s="36"/>
+      <c r="D130" s="36"/>
       <c r="E130" s="0"/>
-      <c r="F130" s="26"/>
+      <c r="F130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="33"/>
-      <c r="B131" s="33"/>
-      <c r="C131" s="33"/>
-      <c r="D131" s="33"/>
+      <c r="A131" s="36"/>
+      <c r="B131" s="36"/>
+      <c r="C131" s="36"/>
+      <c r="D131" s="36"/>
       <c r="E131" s="0"/>
-      <c r="F131" s="26"/>
+      <c r="F131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="33"/>
-      <c r="B132" s="33"/>
-      <c r="C132" s="33"/>
-      <c r="D132" s="33"/>
+      <c r="A132" s="36"/>
+      <c r="B132" s="37"/>
+      <c r="C132" s="37"/>
+      <c r="D132" s="37"/>
       <c r="E132" s="0"/>
-      <c r="F132" s="26"/>
+      <c r="F132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="33"/>
-      <c r="B133" s="33"/>
-      <c r="C133" s="33"/>
-      <c r="D133" s="33"/>
+      <c r="A133" s="36"/>
+      <c r="B133" s="36"/>
+      <c r="C133" s="36"/>
+      <c r="D133" s="36"/>
       <c r="E133" s="0"/>
-      <c r="F133" s="26"/>
+      <c r="F133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="33"/>
-      <c r="B134" s="33"/>
-      <c r="C134" s="33"/>
-      <c r="D134" s="33"/>
+      <c r="A134" s="36"/>
+      <c r="B134" s="36"/>
+      <c r="C134" s="36"/>
+      <c r="D134" s="36"/>
       <c r="E134" s="0"/>
-      <c r="F134" s="26"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="33"/>
-      <c r="B135" s="33"/>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
+      <c r="A135" s="36"/>
+      <c r="B135" s="36"/>
+      <c r="C135" s="36"/>
+      <c r="D135" s="36"/>
       <c r="E135" s="0"/>
-      <c r="F135" s="26"/>
+      <c r="F135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="33"/>
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
+      <c r="A136" s="36"/>
+      <c r="B136" s="37"/>
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
       <c r="E136" s="0"/>
-      <c r="F136" s="26"/>
+      <c r="F136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="33"/>
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
-      <c r="D137" s="33"/>
+      <c r="A137" s="36"/>
+      <c r="B137" s="36"/>
+      <c r="C137" s="36"/>
+      <c r="D137" s="36"/>
       <c r="E137" s="0"/>
-      <c r="F137" s="26"/>
+      <c r="F137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="33"/>
-      <c r="B138" s="33"/>
-      <c r="C138" s="33"/>
-      <c r="D138" s="33"/>
+      <c r="A138" s="36"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
       <c r="E138" s="0"/>
-      <c r="F138" s="26"/>
+      <c r="F138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2477,7 +2469,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="73">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
@@ -2485,6 +2477,7 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B19:D19"/>
@@ -2551,9 +2544,6 @@
     <mergeCell ref="B136:D136"/>
     <mergeCell ref="B138:D138"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="doi:10.5194/gmd-2016-197"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2571,8 +2561,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2592,22 +2582,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" customFormat="false" ht="73.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" customFormat="false" ht="77.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -2615,17 +2605,17 @@
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="0"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="40.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="n">
@@ -2637,17 +2627,17 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="12"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -2655,41 +2645,41 @@
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
-      <c r="B10" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="12"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -2697,67 +2687,67 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="26"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="26"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
-      <c r="B15" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="0"/>
+      <c r="B15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="0"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
-      <c r="B16" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="0"/>
-      <c r="F16" s="26"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="26"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -2765,71 +2755,71 @@
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="n">
         <v>1.2</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="19" t="s">
-        <v>27</v>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="0"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="0"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="26"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="24"/>
+      <c r="B23" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="25"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="26"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="B24" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="0"/>
-      <c r="F24" s="26"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
@@ -2837,79 +2827,79 @@
       <c r="C25" s="0"/>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="0"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="24"/>
+      <c r="B27" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="25"/>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
-      <c r="F27" s="26"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="B28" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="0"/>
-      <c r="F28" s="26"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="0"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="0"/>
-      <c r="F29" s="26"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="26"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="B31" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="26"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
     </row>
@@ -2922,34 +2912,34 @@
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
+      <c r="B34" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="24"/>
+      <c r="A35" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
     </row>
@@ -2962,14 +2952,14 @@
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
+      <c r="B38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
@@ -2977,19 +2967,19 @@
       <c r="A39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="24"/>
+      <c r="B39" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="25"/>
       <c r="D39" s="0"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
@@ -3006,7 +2996,7 @@
         <v>1.3</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -3015,51 +3005,51 @@
     </row>
     <row r="43" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="19" t="s">
-        <v>47</v>
+      <c r="B43" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C43" s="0"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
+      <c r="A45" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="24"/>
+      <c r="A46" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="25"/>
       <c r="D46" s="0"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
@@ -3072,34 +3062,34 @@
       <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="A49" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
+      <c r="A50" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
@@ -3112,34 +3102,34 @@
       <c r="F52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="A53" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
+      <c r="A54" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
@@ -3152,34 +3142,34 @@
       <c r="F56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
+      <c r="A57" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
+      <c r="A58" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
@@ -3192,34 +3182,34 @@
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
+      <c r="A61" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="24"/>
+      <c r="A62" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="25"/>
       <c r="D62" s="0"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
     </row>
@@ -3236,62 +3226,62 @@
         <v>1.4</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="26"/>
+      <c r="F65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="27"/>
-      <c r="B66" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
+      <c r="B66" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="26"/>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="23"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="0"/>
       <c r="E67" s="0"/>
-      <c r="F67" s="26"/>
+      <c r="F67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
+      <c r="A68" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="26"/>
+      <c r="F68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
+      <c r="A69" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="26"/>
+      <c r="F69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="26"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
@@ -3299,39 +3289,39 @@
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
       <c r="E71" s="0"/>
-      <c r="F71" s="26"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
+      <c r="A72" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="26"/>
+      <c r="F72" s="12"/>
     </row>
     <row r="73" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
+      <c r="A73" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="26"/>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
       <c r="E74" s="0"/>
-      <c r="F74" s="26"/>
+      <c r="F74" s="12"/>
     </row>
     <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
@@ -3339,39 +3329,39 @@
       <c r="C75" s="0"/>
       <c r="D75" s="0"/>
       <c r="E75" s="0"/>
-      <c r="F75" s="26"/>
+      <c r="F75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
+      <c r="A76" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
       <c r="E76" s="0"/>
-      <c r="F76" s="26"/>
+      <c r="F76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="24"/>
+      <c r="A77" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="25"/>
       <c r="D77" s="0"/>
       <c r="E77" s="0"/>
-      <c r="F77" s="26"/>
+      <c r="F77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
       <c r="E78" s="0"/>
-      <c r="F78" s="26"/>
+      <c r="F78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
@@ -3379,39 +3369,39 @@
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
       <c r="E79" s="0"/>
-      <c r="F79" s="26"/>
+      <c r="F79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
+      <c r="A80" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="0"/>
-      <c r="F80" s="26"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="24"/>
+      <c r="A81" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="25"/>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
-      <c r="F81" s="26"/>
+      <c r="F81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
       <c r="E82" s="0"/>
-      <c r="F82" s="26"/>
+      <c r="F82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
@@ -3419,15 +3409,15 @@
       <c r="C83" s="0"/>
       <c r="D83" s="0"/>
       <c r="E83" s="0"/>
-      <c r="F83" s="26"/>
+      <c r="F83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
-      <c r="B84" s="0"/>
-      <c r="C84" s="0"/>
-      <c r="D84" s="0"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="0"/>
-      <c r="F84" s="26"/>
+      <c r="F84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0"/>
@@ -3435,15 +3425,15 @@
       <c r="C85" s="0"/>
       <c r="D85" s="0"/>
       <c r="E85" s="0"/>
-      <c r="F85" s="26"/>
+      <c r="F85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
-      <c r="B86" s="0"/>
-      <c r="C86" s="0"/>
-      <c r="D86" s="0"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
       <c r="E86" s="0"/>
-      <c r="F86" s="26"/>
+      <c r="F86" s="12"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
@@ -3451,15 +3441,15 @@
       <c r="C87" s="0"/>
       <c r="D87" s="0"/>
       <c r="E87" s="0"/>
-      <c r="F87" s="26"/>
+      <c r="F87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
-      <c r="B88" s="0"/>
-      <c r="C88" s="0"/>
-      <c r="D88" s="0"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
       <c r="E88" s="0"/>
-      <c r="F88" s="26"/>
+      <c r="F88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0"/>
@@ -3467,15 +3457,15 @@
       <c r="C89" s="0"/>
       <c r="D89" s="0"/>
       <c r="E89" s="0"/>
-      <c r="F89" s="26"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
-      <c r="B90" s="0"/>
-      <c r="C90" s="0"/>
-      <c r="D90" s="0"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
       <c r="E90" s="0"/>
-      <c r="F90" s="26"/>
+      <c r="F90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
@@ -3483,15 +3473,15 @@
       <c r="C91" s="0"/>
       <c r="D91" s="0"/>
       <c r="E91" s="0"/>
-      <c r="F91" s="26"/>
+      <c r="F91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0"/>
-      <c r="B92" s="0"/>
-      <c r="C92" s="0"/>
-      <c r="D92" s="0"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
       <c r="E92" s="0"/>
-      <c r="F92" s="26"/>
+      <c r="F92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
@@ -3499,15 +3489,15 @@
       <c r="C93" s="0"/>
       <c r="D93" s="0"/>
       <c r="E93" s="0"/>
-      <c r="F93" s="26"/>
+      <c r="F93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
-      <c r="B94" s="0"/>
-      <c r="C94" s="0"/>
-      <c r="D94" s="0"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="0"/>
-      <c r="F94" s="26"/>
+      <c r="F94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
@@ -3515,15 +3505,15 @@
       <c r="C95" s="0"/>
       <c r="D95" s="0"/>
       <c r="E95" s="0"/>
-      <c r="F95" s="26"/>
+      <c r="F95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
-      <c r="B96" s="0"/>
-      <c r="C96" s="0"/>
-      <c r="D96" s="0"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
       <c r="E96" s="0"/>
-      <c r="F96" s="26"/>
+      <c r="F96" s="12"/>
     </row>
     <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
@@ -3531,15 +3521,15 @@
       <c r="C97" s="0"/>
       <c r="D97" s="0"/>
       <c r="E97" s="0"/>
-      <c r="F97" s="26"/>
+      <c r="F97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
-      <c r="B98" s="0"/>
-      <c r="C98" s="0"/>
-      <c r="D98" s="0"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
       <c r="E98" s="0"/>
-      <c r="F98" s="26"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
@@ -3547,15 +3537,15 @@
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
       <c r="E99" s="0"/>
-      <c r="F99" s="26"/>
+      <c r="F99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
-      <c r="B100" s="0"/>
-      <c r="C100" s="0"/>
-      <c r="D100" s="0"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
       <c r="E100" s="0"/>
-      <c r="F100" s="26"/>
+      <c r="F100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
@@ -3563,15 +3553,15 @@
       <c r="C101" s="0"/>
       <c r="D101" s="0"/>
       <c r="E101" s="0"/>
-      <c r="F101" s="26"/>
+      <c r="F101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
-      <c r="B102" s="0"/>
-      <c r="C102" s="0"/>
-      <c r="D102" s="0"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
       <c r="E102" s="0"/>
-      <c r="F102" s="26"/>
+      <c r="F102" s="12"/>
     </row>
     <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
@@ -3579,15 +3569,15 @@
       <c r="C103" s="0"/>
       <c r="D103" s="0"/>
       <c r="E103" s="0"/>
-      <c r="F103" s="26"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
-      <c r="B104" s="0"/>
-      <c r="C104" s="0"/>
-      <c r="D104" s="0"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
       <c r="E104" s="0"/>
-      <c r="F104" s="26"/>
+      <c r="F104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0"/>
@@ -3595,15 +3585,15 @@
       <c r="C105" s="0"/>
       <c r="D105" s="0"/>
       <c r="E105" s="0"/>
-      <c r="F105" s="26"/>
+      <c r="F105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0"/>
-      <c r="B106" s="0"/>
-      <c r="C106" s="0"/>
-      <c r="D106" s="0"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
       <c r="E106" s="0"/>
-      <c r="F106" s="26"/>
+      <c r="F106" s="12"/>
     </row>
     <row r="107" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0"/>
@@ -3611,15 +3601,15 @@
       <c r="C107" s="0"/>
       <c r="D107" s="0"/>
       <c r="E107" s="0"/>
-      <c r="F107" s="26"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0"/>
-      <c r="B108" s="0"/>
-      <c r="C108" s="0"/>
-      <c r="D108" s="0"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
       <c r="E108" s="0"/>
-      <c r="F108" s="26"/>
+      <c r="F108" s="12"/>
     </row>
     <row r="109" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0"/>
@@ -3627,15 +3617,15 @@
       <c r="C109" s="0"/>
       <c r="D109" s="0"/>
       <c r="E109" s="0"/>
-      <c r="F109" s="26"/>
+      <c r="F109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0"/>
-      <c r="B110" s="0"/>
-      <c r="C110" s="0"/>
-      <c r="D110" s="0"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
       <c r="E110" s="0"/>
-      <c r="F110" s="26"/>
+      <c r="F110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0"/>
@@ -3643,15 +3633,15 @@
       <c r="C111" s="0"/>
       <c r="D111" s="0"/>
       <c r="E111" s="0"/>
-      <c r="F111" s="26"/>
+      <c r="F111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0"/>
-      <c r="B112" s="0"/>
-      <c r="C112" s="0"/>
-      <c r="D112" s="0"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
       <c r="E112" s="0"/>
-      <c r="F112" s="26"/>
+      <c r="F112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0"/>
@@ -3659,206 +3649,206 @@
       <c r="C113" s="0"/>
       <c r="D113" s="0"/>
       <c r="E113" s="0"/>
-      <c r="F113" s="26"/>
+      <c r="F113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
-      <c r="B114" s="0"/>
-      <c r="C114" s="0"/>
-      <c r="D114" s="0"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
       <c r="E114" s="0"/>
-      <c r="F114" s="26"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
       <c r="B115" s="0"/>
       <c r="C115" s="0"/>
       <c r="D115" s="0"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="26"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0"/>
-      <c r="B116" s="0"/>
-      <c r="C116" s="0"/>
-      <c r="D116" s="0"/>
-      <c r="F116" s="26"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="33"/>
-      <c r="B117" s="33"/>
-      <c r="C117" s="33"/>
-      <c r="D117" s="33"/>
+      <c r="A117" s="36"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="36"/>
+      <c r="D117" s="36"/>
       <c r="E117" s="0"/>
-      <c r="F117" s="26"/>
+      <c r="F117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="33"/>
-      <c r="B118" s="33"/>
-      <c r="C118" s="33"/>
-      <c r="D118" s="33"/>
+      <c r="A118" s="36"/>
+      <c r="B118" s="36"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
       <c r="E118" s="0"/>
-      <c r="F118" s="26"/>
+      <c r="F118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="33"/>
-      <c r="B119" s="33"/>
-      <c r="C119" s="33"/>
-      <c r="D119" s="33"/>
+      <c r="A119" s="36"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="37"/>
       <c r="E119" s="0"/>
-      <c r="F119" s="26"/>
+      <c r="F119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="33"/>
-      <c r="B120" s="33"/>
-      <c r="C120" s="33"/>
-      <c r="D120" s="33"/>
+      <c r="A120" s="36"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="36"/>
+      <c r="D120" s="36"/>
       <c r="E120" s="0"/>
-      <c r="F120" s="26"/>
+      <c r="F120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="33"/>
-      <c r="B121" s="33"/>
-      <c r="C121" s="33"/>
-      <c r="D121" s="33"/>
+      <c r="A121" s="36"/>
+      <c r="B121" s="37"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="37"/>
       <c r="E121" s="0"/>
-      <c r="F121" s="26"/>
+      <c r="F121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="33"/>
-      <c r="B122" s="33"/>
-      <c r="C122" s="33"/>
-      <c r="D122" s="33"/>
+      <c r="A122" s="36"/>
+      <c r="B122" s="36"/>
+      <c r="C122" s="36"/>
+      <c r="D122" s="36"/>
       <c r="E122" s="0"/>
-      <c r="F122" s="26"/>
+      <c r="F122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="33"/>
-      <c r="B123" s="33"/>
-      <c r="C123" s="33"/>
-      <c r="D123" s="33"/>
+      <c r="A123" s="36"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="36"/>
+      <c r="D123" s="36"/>
       <c r="E123" s="0"/>
-      <c r="F123" s="26"/>
+      <c r="F123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="33"/>
-      <c r="B124" s="33"/>
-      <c r="C124" s="33"/>
-      <c r="D124" s="33"/>
+      <c r="A124" s="36"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="37"/>
+      <c r="D124" s="37"/>
       <c r="E124" s="0"/>
-      <c r="F124" s="26"/>
+      <c r="F124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="33"/>
-      <c r="B125" s="33"/>
-      <c r="C125" s="33"/>
-      <c r="D125" s="33"/>
+      <c r="A125" s="36"/>
+      <c r="B125" s="36"/>
+      <c r="C125" s="36"/>
+      <c r="D125" s="36"/>
       <c r="E125" s="0"/>
-      <c r="F125" s="26"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="33"/>
-      <c r="B126" s="33"/>
-      <c r="C126" s="33"/>
-      <c r="D126" s="33"/>
+      <c r="A126" s="36"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="37"/>
+      <c r="D126" s="37"/>
       <c r="E126" s="0"/>
-      <c r="F126" s="26"/>
+      <c r="F126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="33"/>
-      <c r="B127" s="33"/>
-      <c r="C127" s="33"/>
-      <c r="D127" s="33"/>
+      <c r="A127" s="36"/>
+      <c r="B127" s="36"/>
+      <c r="C127" s="36"/>
+      <c r="D127" s="36"/>
       <c r="E127" s="0"/>
-      <c r="F127" s="26"/>
+      <c r="F127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="33"/>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33"/>
-      <c r="D128" s="33"/>
+      <c r="A128" s="36"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
       <c r="E128" s="0"/>
-      <c r="F128" s="26"/>
+      <c r="F128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="33"/>
-      <c r="B129" s="33"/>
-      <c r="C129" s="33"/>
-      <c r="D129" s="33"/>
+      <c r="A129" s="36"/>
+      <c r="B129" s="36"/>
+      <c r="C129" s="36"/>
+      <c r="D129" s="36"/>
       <c r="E129" s="0"/>
-      <c r="F129" s="26"/>
+      <c r="F129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="33"/>
-      <c r="B130" s="33"/>
-      <c r="C130" s="33"/>
-      <c r="D130" s="33"/>
+      <c r="A130" s="36"/>
+      <c r="B130" s="36"/>
+      <c r="C130" s="36"/>
+      <c r="D130" s="36"/>
       <c r="E130" s="0"/>
-      <c r="F130" s="26"/>
+      <c r="F130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="33"/>
-      <c r="B131" s="33"/>
-      <c r="C131" s="33"/>
-      <c r="D131" s="33"/>
+      <c r="A131" s="36"/>
+      <c r="B131" s="36"/>
+      <c r="C131" s="36"/>
+      <c r="D131" s="36"/>
       <c r="E131" s="0"/>
-      <c r="F131" s="26"/>
+      <c r="F131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="33"/>
-      <c r="B132" s="33"/>
-      <c r="C132" s="33"/>
-      <c r="D132" s="33"/>
+      <c r="A132" s="36"/>
+      <c r="B132" s="37"/>
+      <c r="C132" s="37"/>
+      <c r="D132" s="37"/>
       <c r="E132" s="0"/>
-      <c r="F132" s="26"/>
+      <c r="F132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="33"/>
-      <c r="B133" s="33"/>
-      <c r="C133" s="33"/>
-      <c r="D133" s="33"/>
+      <c r="A133" s="36"/>
+      <c r="B133" s="36"/>
+      <c r="C133" s="36"/>
+      <c r="D133" s="36"/>
       <c r="E133" s="0"/>
-      <c r="F133" s="26"/>
+      <c r="F133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="33"/>
-      <c r="B134" s="33"/>
-      <c r="C134" s="33"/>
-      <c r="D134" s="33"/>
+      <c r="A134" s="36"/>
+      <c r="B134" s="36"/>
+      <c r="C134" s="36"/>
+      <c r="D134" s="36"/>
       <c r="E134" s="0"/>
-      <c r="F134" s="26"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="33"/>
-      <c r="B135" s="33"/>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
+      <c r="A135" s="36"/>
+      <c r="B135" s="36"/>
+      <c r="C135" s="36"/>
+      <c r="D135" s="36"/>
       <c r="E135" s="0"/>
-      <c r="F135" s="26"/>
+      <c r="F135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="33"/>
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
+      <c r="A136" s="36"/>
+      <c r="B136" s="37"/>
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
       <c r="E136" s="0"/>
-      <c r="F136" s="26"/>
+      <c r="F136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="33"/>
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
-      <c r="D137" s="33"/>
+      <c r="A137" s="36"/>
+      <c r="B137" s="36"/>
+      <c r="C137" s="36"/>
+      <c r="D137" s="36"/>
       <c r="E137" s="0"/>
-      <c r="F137" s="26"/>
+      <c r="F137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="33"/>
-      <c r="B138" s="33"/>
-      <c r="C138" s="33"/>
-      <c r="D138" s="33"/>
+      <c r="A138" s="36"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
       <c r="E138" s="0"/>
-      <c r="F138" s="26"/>
+      <c r="F138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4128,7 +4118,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="73">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
@@ -4136,6 +4126,7 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B19:D19"/>
@@ -4202,9 +4193,6 @@
     <mergeCell ref="B136:D136"/>
     <mergeCell ref="B138:D138"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="doi:10.5194/gmd-2016-197"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1. Clarify nature of example tab by name and title
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ocean of HadGEM3-GC3.1 N512 ORCA12 on ARCHER-XC30_2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Example" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="&lt;realm name&gt; of &lt;model name&gt; on &lt;machine name&gt;" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">Internal notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Performance of ARCHER-XC30 for the ocean realm of model HadGEM3-GC3.1 N512 ORCA12</t>
+    <t xml:space="preserve">(EXAMPLE) Performance of ARCHER-XC30 for the ocean realm of model HadGEM3-GC3.1 N512 ORCA12</t>
   </si>
   <si>
     <t xml:space="preserve">Describes the properties of a performance of a configured model on a particular system/machine. Based on "CPMIP: Measurements of Real Computational Performance of Earth System Models" (Balaji et. al. 2016, doi:10.5194/gmd-2016-197).</t>
@@ -762,7 +762,7 @@
   </sheetPr>
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -899,8 +899,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
1. Address feedback about style of pre-determined items
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Example" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Example, realm-specific" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="&lt;realm name&gt; of &lt;model name&gt; on &lt;machine name&gt;" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machine Performance</t>
   </si>
@@ -95,6 +95,30 @@
     <t xml:space="preserve">1.1.2 *</t>
   </si>
   <si>
+    <t xml:space="preserve">Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform on which performance was tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCHER-XC30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.3 *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model for which performance was tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HadGEM3-GC3.1 N512 ORCA12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.4 *</t>
+  </si>
+  <si>
     <t xml:space="preserve">Realm</t>
   </si>
   <si>
@@ -113,54 +137,30 @@
     <t xml:space="preserve">Metrics describing the model and the platform.</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.1 *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platform on which performance was tested.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARCHER-XC30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.2 *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model for which performance was tested.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HadGEM3-GC3.1 N512 ORCA12</t>
+    <t xml:space="preserve">1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution measured as the number of gridpoints (or more generally, spatial degrees of freedom) NX x NY x NZ per component with an independent discretization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complexity measured as the number of prognostic variables per component with an independent discretization.</t>
   </si>
   <si>
     <t xml:space="preserve">1.2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTEGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution measured as the number of gridpoints (or more generally, spatial degrees of freedom) NX x NY x NZ per component with an independent discretization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complexity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complexity measured as the number of prognostic variables per component with an independent discretization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Compiler</t>
   </si>
   <si>
@@ -212,73 +212,76 @@
     <t xml:space="preserve">Joules per simulated year</t>
   </si>
   <si>
+    <t xml:space="preserve">The energy cost of a simulation, measured in joules per simulated year (JPSY). Given the energy E in joules consumed over a budgeting interval T (generally 1 month or 1 year, in units of hours), JPSY=CHSY*E*T/NP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallelisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or or all cores were used all of the time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further detail: CPMIP Metrics: Coupling, memory and I/O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information about how the various components of performance were related; set of additional information related to coupling, memory and I/O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupling cost measures the overhead caused by coupling. This can include the cost of the coupling algorithm itself (which may involve grid interpolation and computation of transfer coefficients for conservative coupling) as well as load imbalance. It is the normalized difference between the time-processor integral for the whole model versus the sum of individual concurrent components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory bloat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size to the ideal memory size (the size of the complete model state, which in theory is all you need to hold in memory)Mi, defined below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data output cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data output cost is the cost of performing I/O, and is the ratio of CHSY with and without I/O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data intensity the amount of data produced per compute-hour, in units GB per compute-hour.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance of &lt;machine name&gt; for the &lt;realm name&gt; realm of model &lt;model name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;machine name&gt; representative performance for the &lt;realm name&gt; realm of model &lt;model name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;machine name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;model name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;realm name&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">The energy cost of a simulation, measured in joules per simulated year (JPSY). Given the energy E in joules consumed over a budgeting interval T (generally 1 month or 1 year, in units of hours), JPSY=CHSY*E*T/NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallelisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or or all cores were used all of the time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further detail: CPMIP Metrics: Coupling, memory and I/O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information about how the various components of performance were related; set of additional information related to coupling, memory and I/O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupling cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupling cost measures the overhead caused by coupling. This can include the cost of the coupling algorithm itself (which may involve grid interpolation and computation of transfer coefficients for conservative coupling) as well as load imbalance. It is the normalized difference between the time-processor integral for the whole model versus the sum of individual concurrent components.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory bloat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size to the ideal memory size (the size of the complete model state, which in theory is all you need to hold in memory)Mi, defined below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data output cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data output cost is the cost of performing I/O, and is the ratio of CHSY with and without I/O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data intensity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data intensity the amount of data produced per compute-hour, in units GB per compute-hour.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance of &lt;machine name&gt; for the &lt;realm name&gt; realm of model &lt;model name&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;machine name&gt; representative performance for the &lt;realm name&gt; realm of model &lt;model name&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;realm name&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;machine name&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;model name&gt;</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -401,7 +404,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
@@ -425,6 +428,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -433,7 +443,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +460,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF003366"/>
         <bgColor rgb="FF333399"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF111111"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -534,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -615,6 +643,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,11 +659,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -639,12 +675,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -655,7 +695,7 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,12 +703,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -744,7 +792,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -763,7 +811,7 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,7 +948,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -955,27 +1003,27 @@
       <c r="E4" s="0"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" customFormat="false" ht="40.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="n">
+    <row r="5" customFormat="false" ht="41.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="n">
         <v>1.1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="21"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="18"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -983,41 +1031,41 @@
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="18"/>
+      <c r="F7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="18"/>
+      <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="18"/>
+      <c r="F10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -1025,213 +1073,213 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="27"/>
+      <c r="F11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="27"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="0"/>
+      <c r="F13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="27"/>
+      <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="25"/>
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
-      <c r="F15" s="27"/>
+      <c r="F15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="B16" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="0"/>
-      <c r="F16" s="27"/>
+      <c r="F16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
+      <c r="A17" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="F17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="0"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
-      <c r="B19" s="20" t="s">
-        <v>28</v>
-      </c>
+      <c r="B19" s="0"/>
       <c r="C19" s="0"/>
-      <c r="D19" s="21"/>
+      <c r="D19" s="0"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="21"/>
+      <c r="A20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+      <c r="A21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="0"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="27"/>
+      <c r="F22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="27"/>
-    </row>
-    <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
+      <c r="B24" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="0"/>
-      <c r="F24" s="27"/>
+      <c r="F24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
       <c r="E25" s="0"/>
-      <c r="F25" s="27"/>
-    </row>
-    <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="25" t="s">
+      <c r="F25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="0"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="0"/>
-      <c r="F26" s="27"/>
+      <c r="F26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="0"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="20"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="0"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="0"/>
-      <c r="F28" s="27"/>
+      <c r="F28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="0"/>
-      <c r="F29" s="27"/>
-    </row>
-    <row r="30" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="s">
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30" t="n">
+      <c r="A31" s="32"/>
+      <c r="B31" s="33" t="n">
         <v>1168884900</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
     </row>
@@ -1244,36 +1292,36 @@
       <c r="F32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="30" t="n">
+      <c r="B35" s="33" t="n">
         <v>18</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
     </row>
@@ -1286,36 +1334,36 @@
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="25"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="0"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
@@ -1341,53 +1389,53 @@
     </row>
     <row r="42" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="0"/>
-      <c r="D42" s="21"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="0"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="26" t="n">
+      <c r="B46" s="35" t="n">
         <v>0.49</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
@@ -1400,36 +1448,36 @@
       <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="B50" s="30" t="n">
+      <c r="B50" s="33" t="n">
         <v>0.34</v>
       </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
@@ -1442,36 +1490,36 @@
       <c r="F51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
-      <c r="B54" s="30" t="n">
+      <c r="B54" s="33" t="n">
         <v>585540</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
@@ -1484,36 +1532,36 @@
       <c r="F55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
-      <c r="B58" s="33" t="n">
+      <c r="B58" s="37" t="n">
         <v>23000000000</v>
       </c>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
@@ -1526,36 +1574,36 @@
       <c r="F59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="25"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
-      <c r="B62" s="26" t="n">
+      <c r="B62" s="35" t="n">
         <v>12024</v>
       </c>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
@@ -1577,57 +1625,57 @@
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
       <c r="E64" s="0"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="38"/>
     </row>
     <row r="65" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="27"/>
+      <c r="F65" s="38"/>
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="0"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="27"/>
+      <c r="F66" s="38"/>
     </row>
     <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="0"/>
-      <c r="F67" s="27"/>
+      <c r="F67" s="38"/>
     </row>
     <row r="68" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="27"/>
+      <c r="F68" s="38"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="27"/>
+      <c r="F69" s="38"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
@@ -1635,41 +1683,41 @@
       <c r="C70" s="0"/>
       <c r="D70" s="0"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="27"/>
+      <c r="F70" s="38"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="0"/>
-      <c r="F71" s="27"/>
+      <c r="F71" s="38"/>
     </row>
     <row r="72" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="27"/>
+      <c r="F72" s="38"/>
     </row>
     <row r="73" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
-      <c r="B73" s="26" t="n">
+      <c r="B73" s="35" t="n">
         <v>183</v>
       </c>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="27"/>
+      <c r="F73" s="38"/>
     </row>
     <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
@@ -1677,39 +1725,39 @@
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
       <c r="E74" s="0"/>
-      <c r="F74" s="27"/>
+      <c r="F74" s="38"/>
     </row>
     <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="0"/>
-      <c r="F75" s="27"/>
+      <c r="F75" s="38"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24" t="s">
+      <c r="A76" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C76" s="25"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
-      <c r="F76" s="27"/>
+      <c r="F76" s="38"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
       <c r="E77" s="0"/>
-      <c r="F77" s="27"/>
+      <c r="F77" s="38"/>
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
@@ -1717,41 +1765,41 @@
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
       <c r="E78" s="0"/>
-      <c r="F78" s="27"/>
+      <c r="F78" s="38"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="0"/>
-      <c r="F79" s="27"/>
+      <c r="F79" s="38"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="24" t="s">
+      <c r="A80" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="B80" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="25"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="0"/>
       <c r="E80" s="0"/>
-      <c r="F80" s="27"/>
+      <c r="F80" s="38"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0"/>
-      <c r="B81" s="26" t="n">
+      <c r="B81" s="35" t="n">
         <v>207</v>
       </c>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
       <c r="E81" s="0"/>
-      <c r="F81" s="27"/>
+      <c r="F81" s="38"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
@@ -1759,15 +1807,15 @@
       <c r="C82" s="0"/>
       <c r="D82" s="0"/>
       <c r="E82" s="0"/>
-      <c r="F82" s="27"/>
+      <c r="F82" s="38"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="0"/>
-      <c r="F83" s="27"/>
+      <c r="F83" s="38"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
@@ -1775,15 +1823,15 @@
       <c r="C84" s="0"/>
       <c r="D84" s="0"/>
       <c r="E84" s="0"/>
-      <c r="F84" s="27"/>
+      <c r="F84" s="38"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
       <c r="E85" s="0"/>
-      <c r="F85" s="27"/>
+      <c r="F85" s="38"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
@@ -1791,15 +1839,15 @@
       <c r="C86" s="0"/>
       <c r="D86" s="0"/>
       <c r="E86" s="0"/>
-      <c r="F86" s="27"/>
+      <c r="F86" s="38"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
-      <c r="D87" s="34"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
       <c r="E87" s="0"/>
-      <c r="F87" s="27"/>
+      <c r="F87" s="38"/>
     </row>
     <row r="88" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
@@ -1807,15 +1855,15 @@
       <c r="C88" s="0"/>
       <c r="D88" s="0"/>
       <c r="E88" s="0"/>
-      <c r="F88" s="27"/>
+      <c r="F88" s="38"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
       <c r="E89" s="0"/>
-      <c r="F89" s="27"/>
+      <c r="F89" s="38"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
@@ -1823,15 +1871,15 @@
       <c r="C90" s="0"/>
       <c r="D90" s="0"/>
       <c r="E90" s="0"/>
-      <c r="F90" s="27"/>
+      <c r="F90" s="38"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
       <c r="E91" s="0"/>
-      <c r="F91" s="27"/>
+      <c r="F91" s="38"/>
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0"/>
@@ -1839,15 +1887,15 @@
       <c r="C92" s="0"/>
       <c r="D92" s="0"/>
       <c r="E92" s="0"/>
-      <c r="F92" s="27"/>
+      <c r="F92" s="38"/>
     </row>
     <row r="93" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
       <c r="E93" s="0"/>
-      <c r="F93" s="27"/>
+      <c r="F93" s="38"/>
     </row>
     <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
@@ -1855,15 +1903,15 @@
       <c r="C94" s="0"/>
       <c r="D94" s="0"/>
       <c r="E94" s="0"/>
-      <c r="F94" s="27"/>
+      <c r="F94" s="38"/>
     </row>
     <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="34"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
       <c r="E95" s="0"/>
-      <c r="F95" s="27"/>
+      <c r="F95" s="38"/>
     </row>
     <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
@@ -1871,15 +1919,15 @@
       <c r="C96" s="0"/>
       <c r="D96" s="0"/>
       <c r="E96" s="0"/>
-      <c r="F96" s="27"/>
+      <c r="F96" s="38"/>
     </row>
     <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="34"/>
-      <c r="D97" s="34"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
       <c r="E97" s="0"/>
-      <c r="F97" s="27"/>
+      <c r="F97" s="38"/>
     </row>
     <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
@@ -1887,15 +1935,15 @@
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
       <c r="E98" s="0"/>
-      <c r="F98" s="27"/>
+      <c r="F98" s="38"/>
     </row>
     <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
-      <c r="B99" s="34"/>
-      <c r="C99" s="34"/>
-      <c r="D99" s="34"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
       <c r="E99" s="0"/>
-      <c r="F99" s="27"/>
+      <c r="F99" s="38"/>
     </row>
     <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
@@ -1903,15 +1951,15 @@
       <c r="C100" s="0"/>
       <c r="D100" s="0"/>
       <c r="E100" s="0"/>
-      <c r="F100" s="27"/>
+      <c r="F100" s="38"/>
     </row>
     <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
-      <c r="B101" s="34"/>
-      <c r="C101" s="34"/>
-      <c r="D101" s="34"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
       <c r="E101" s="0"/>
-      <c r="F101" s="27"/>
+      <c r="F101" s="38"/>
     </row>
     <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
@@ -1919,15 +1967,15 @@
       <c r="C102" s="0"/>
       <c r="D102" s="0"/>
       <c r="E102" s="0"/>
-      <c r="F102" s="27"/>
+      <c r="F102" s="38"/>
     </row>
     <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
-      <c r="B103" s="34"/>
-      <c r="C103" s="34"/>
-      <c r="D103" s="34"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
       <c r="E103" s="0"/>
-      <c r="F103" s="27"/>
+      <c r="F103" s="38"/>
     </row>
     <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
@@ -1935,15 +1983,15 @@
       <c r="C104" s="0"/>
       <c r="D104" s="0"/>
       <c r="E104" s="0"/>
-      <c r="F104" s="27"/>
+      <c r="F104" s="38"/>
     </row>
     <row r="105" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0"/>
-      <c r="B105" s="34"/>
-      <c r="C105" s="34"/>
-      <c r="D105" s="34"/>
+      <c r="B105" s="39"/>
+      <c r="C105" s="39"/>
+      <c r="D105" s="39"/>
       <c r="E105" s="0"/>
-      <c r="F105" s="27"/>
+      <c r="F105" s="38"/>
     </row>
     <row r="106" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0"/>
@@ -1951,15 +1999,15 @@
       <c r="C106" s="0"/>
       <c r="D106" s="0"/>
       <c r="E106" s="0"/>
-      <c r="F106" s="27"/>
+      <c r="F106" s="38"/>
     </row>
     <row r="107" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0"/>
-      <c r="B107" s="34"/>
-      <c r="C107" s="34"/>
-      <c r="D107" s="34"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="39"/>
+      <c r="D107" s="39"/>
       <c r="E107" s="0"/>
-      <c r="F107" s="27"/>
+      <c r="F107" s="38"/>
     </row>
     <row r="108" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0"/>
@@ -1967,15 +2015,15 @@
       <c r="C108" s="0"/>
       <c r="D108" s="0"/>
       <c r="E108" s="0"/>
-      <c r="F108" s="27"/>
+      <c r="F108" s="38"/>
     </row>
     <row r="109" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0"/>
-      <c r="B109" s="34"/>
-      <c r="C109" s="34"/>
-      <c r="D109" s="34"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="39"/>
       <c r="E109" s="0"/>
-      <c r="F109" s="27"/>
+      <c r="F109" s="38"/>
     </row>
     <row r="110" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0"/>
@@ -1983,15 +2031,15 @@
       <c r="C110" s="0"/>
       <c r="D110" s="0"/>
       <c r="E110" s="0"/>
-      <c r="F110" s="27"/>
+      <c r="F110" s="38"/>
     </row>
     <row r="111" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0"/>
-      <c r="B111" s="34"/>
-      <c r="C111" s="34"/>
-      <c r="D111" s="34"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
       <c r="E111" s="0"/>
-      <c r="F111" s="27"/>
+      <c r="F111" s="38"/>
     </row>
     <row r="112" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0"/>
@@ -1999,206 +2047,206 @@
       <c r="C112" s="0"/>
       <c r="D112" s="0"/>
       <c r="E112" s="0"/>
-      <c r="F112" s="27"/>
+      <c r="F112" s="38"/>
     </row>
     <row r="113" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0"/>
-      <c r="B113" s="34"/>
-      <c r="C113" s="34"/>
-      <c r="D113" s="34"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
       <c r="E113" s="0"/>
-      <c r="F113" s="27"/>
+      <c r="F113" s="38"/>
     </row>
     <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
       <c r="B114" s="0"/>
       <c r="C114" s="0"/>
       <c r="D114" s="0"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
     </row>
     <row r="115" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
-      <c r="B115" s="34"/>
-      <c r="C115" s="34"/>
-      <c r="D115" s="34"/>
-      <c r="F115" s="27"/>
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="39"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="35"/>
-      <c r="B116" s="35"/>
-      <c r="C116" s="35"/>
-      <c r="D116" s="35"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="0"/>
-      <c r="F116" s="27"/>
+      <c r="F116" s="38"/>
     </row>
     <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="35"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
-      <c r="D117" s="35"/>
+      <c r="A117" s="40"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
+      <c r="D117" s="40"/>
       <c r="E117" s="0"/>
-      <c r="F117" s="27"/>
+      <c r="F117" s="38"/>
     </row>
     <row r="118" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="35"/>
-      <c r="B118" s="36"/>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
+      <c r="A118" s="40"/>
+      <c r="B118" s="41"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
       <c r="E118" s="0"/>
-      <c r="F118" s="27"/>
+      <c r="F118" s="38"/>
     </row>
     <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="35"/>
-      <c r="B119" s="35"/>
-      <c r="C119" s="35"/>
-      <c r="D119" s="35"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="0"/>
-      <c r="F119" s="27"/>
+      <c r="F119" s="38"/>
     </row>
     <row r="120" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="35"/>
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
+      <c r="A120" s="40"/>
+      <c r="B120" s="41"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
       <c r="E120" s="0"/>
-      <c r="F120" s="27"/>
+      <c r="F120" s="38"/>
     </row>
     <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="35"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
-      <c r="D121" s="35"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
-      <c r="F121" s="27"/>
+      <c r="F121" s="38"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="35"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
-      <c r="D122" s="35"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
       <c r="E122" s="0"/>
-      <c r="F122" s="27"/>
+      <c r="F122" s="38"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="35"/>
-      <c r="B123" s="36"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="41"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
       <c r="E123" s="0"/>
-      <c r="F123" s="27"/>
+      <c r="F123" s="38"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="35"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="35"/>
-      <c r="D124" s="35"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
       <c r="E124" s="0"/>
-      <c r="F124" s="27"/>
+      <c r="F124" s="38"/>
     </row>
     <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="35"/>
-      <c r="B125" s="36"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
+      <c r="A125" s="40"/>
+      <c r="B125" s="41"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="41"/>
       <c r="E125" s="0"/>
-      <c r="F125" s="27"/>
+      <c r="F125" s="38"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="35"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35"/>
-      <c r="D126" s="35"/>
+      <c r="A126" s="40"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
+      <c r="D126" s="40"/>
       <c r="E126" s="0"/>
-      <c r="F126" s="27"/>
+      <c r="F126" s="38"/>
     </row>
     <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="35"/>
-      <c r="B127" s="36"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="41"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
       <c r="E127" s="0"/>
-      <c r="F127" s="27"/>
+      <c r="F127" s="38"/>
     </row>
     <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="35"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="35"/>
-      <c r="D128" s="35"/>
+      <c r="A128" s="40"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
-      <c r="F128" s="27"/>
+      <c r="F128" s="38"/>
     </row>
     <row r="129" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="35"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="35"/>
-      <c r="D129" s="35"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="40"/>
+      <c r="C129" s="40"/>
+      <c r="D129" s="40"/>
       <c r="E129" s="0"/>
-      <c r="F129" s="27"/>
+      <c r="F129" s="38"/>
     </row>
     <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="35"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="35"/>
-      <c r="D130" s="35"/>
+      <c r="A130" s="40"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="40"/>
       <c r="E130" s="0"/>
-      <c r="F130" s="27"/>
+      <c r="F130" s="38"/>
     </row>
     <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="35"/>
-      <c r="B131" s="36"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="41"/>
+      <c r="C131" s="41"/>
+      <c r="D131" s="41"/>
       <c r="E131" s="0"/>
-      <c r="F131" s="27"/>
+      <c r="F131" s="38"/>
     </row>
     <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="35"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="35"/>
-      <c r="D132" s="35"/>
+      <c r="A132" s="40"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="40"/>
+      <c r="D132" s="40"/>
       <c r="E132" s="0"/>
-      <c r="F132" s="27"/>
+      <c r="F132" s="38"/>
     </row>
     <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="35"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="35"/>
-      <c r="D133" s="35"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="40"/>
+      <c r="D133" s="40"/>
       <c r="E133" s="0"/>
-      <c r="F133" s="27"/>
+      <c r="F133" s="38"/>
     </row>
     <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="35"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="35"/>
-      <c r="D134" s="35"/>
+      <c r="A134" s="40"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="40"/>
+      <c r="D134" s="40"/>
       <c r="E134" s="0"/>
-      <c r="F134" s="27"/>
+      <c r="F134" s="38"/>
     </row>
     <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="35"/>
-      <c r="B135" s="36"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="36"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="41"/>
+      <c r="C135" s="41"/>
+      <c r="D135" s="41"/>
       <c r="E135" s="0"/>
-      <c r="F135" s="27"/>
+      <c r="F135" s="38"/>
     </row>
     <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="35"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="35"/>
-      <c r="D136" s="35"/>
+      <c r="A136" s="40"/>
+      <c r="B136" s="40"/>
+      <c r="C136" s="40"/>
+      <c r="D136" s="40"/>
       <c r="E136" s="0"/>
-      <c r="F136" s="27"/>
+      <c r="F136" s="38"/>
     </row>
     <row r="137" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="35"/>
-      <c r="B137" s="36"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="36"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="41"/>
+      <c r="C137" s="41"/>
+      <c r="D137" s="41"/>
       <c r="E137" s="0"/>
-      <c r="F137" s="27"/>
+      <c r="F137" s="38"/>
     </row>
     <row r="138" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2477,12 +2525,12 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
@@ -2542,9 +2590,6 @@
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B137:D137"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" display="Note: corresponds to one of the realms defined at https://github.com/WCRP-CMIP/CMIP6_CVs/blob/master/CMIP6_realm.json."/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2563,7 +2608,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2619,24 +2664,24 @@
       <c r="F4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="40.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="n">
+      <c r="A5" s="20" t="n">
         <v>1.1</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="0"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="21"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="0"/>
       <c r="F6" s="18"/>
     </row>
@@ -2649,36 +2694,36 @@
       <c r="F7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="0"/>
       <c r="F8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="0"/>
       <c r="F10" s="18"/>
     </row>
@@ -2688,211 +2733,211 @@
       <c r="C11" s="0"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="27"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="27"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="0"/>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="27"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="25"/>
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
-      <c r="F15" s="27"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="A16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="0"/>
-      <c r="F16" s="27"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
+      <c r="A17" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="0"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
-      <c r="B19" s="20" t="s">
-        <v>28</v>
-      </c>
+      <c r="B19" s="0"/>
       <c r="C19" s="0"/>
-      <c r="D19" s="21"/>
+      <c r="D19" s="0"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="21"/>
+      <c r="A20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+      <c r="A21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="0"/>
       <c r="E21" s="0"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
-      <c r="F22" s="27"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="0"/>
       <c r="E23" s="0"/>
-      <c r="F23" s="27"/>
-    </row>
-    <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F23" s="38"/>
+    </row>
+    <row r="24" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
+      <c r="B24" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="0"/>
-      <c r="F24" s="27"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
       <c r="E25" s="0"/>
-      <c r="F25" s="27"/>
-    </row>
-    <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="25" t="s">
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="0"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="0"/>
-      <c r="F26" s="27"/>
-    </row>
-    <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F26" s="38"/>
+    </row>
+    <row r="27" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="B27" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="0"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="0"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="20"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="0"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="0"/>
-      <c r="F28" s="27"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="0"/>
-      <c r="F29" s="27"/>
+      <c r="F29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
     </row>
@@ -2905,34 +2950,34 @@
       <c r="F32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
     </row>
@@ -2945,34 +2990,34 @@
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="25"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="0"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
@@ -2998,51 +3043,51 @@
     </row>
     <row r="42" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="0"/>
-      <c r="D42" s="21"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="0"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
@@ -3055,34 +3100,34 @@
       <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
@@ -3095,34 +3140,34 @@
       <c r="F51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
@@ -3135,34 +3180,34 @@
       <c r="F55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
+      <c r="B57" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
@@ -3175,34 +3220,34 @@
       <c r="F59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="25"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
@@ -3224,57 +3269,57 @@
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
       <c r="E64" s="0"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="38"/>
     </row>
     <row r="65" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31"/>
+      <c r="A65" s="34"/>
       <c r="B65" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="27"/>
+      <c r="F65" s="38"/>
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="0"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="27"/>
+      <c r="F66" s="38"/>
     </row>
     <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="0"/>
-      <c r="F67" s="27"/>
+      <c r="F67" s="38"/>
     </row>
     <row r="68" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="27"/>
+      <c r="F68" s="38"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="27"/>
+      <c r="F69" s="38"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
@@ -3282,39 +3327,39 @@
       <c r="C70" s="0"/>
       <c r="D70" s="0"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="27"/>
+      <c r="F70" s="38"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="0"/>
-      <c r="F71" s="27"/>
+      <c r="F71" s="38"/>
     </row>
     <row r="72" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="27"/>
+      <c r="F72" s="38"/>
     </row>
     <row r="73" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="27"/>
+      <c r="F73" s="38"/>
     </row>
     <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
@@ -3322,39 +3367,39 @@
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
       <c r="E74" s="0"/>
-      <c r="F74" s="27"/>
+      <c r="F74" s="38"/>
     </row>
     <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="0"/>
-      <c r="F75" s="27"/>
+      <c r="F75" s="38"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24" t="s">
+      <c r="A76" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C76" s="25"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
-      <c r="F76" s="27"/>
+      <c r="F76" s="38"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
       <c r="E77" s="0"/>
-      <c r="F77" s="27"/>
+      <c r="F77" s="38"/>
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
@@ -3362,39 +3407,39 @@
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
       <c r="E78" s="0"/>
-      <c r="F78" s="27"/>
+      <c r="F78" s="38"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="0"/>
-      <c r="F79" s="27"/>
+      <c r="F79" s="38"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="24" t="s">
+      <c r="A80" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="B80" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="25"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="0"/>
       <c r="E80" s="0"/>
-      <c r="F80" s="27"/>
+      <c r="F80" s="38"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
       <c r="E81" s="0"/>
-      <c r="F81" s="27"/>
+      <c r="F81" s="38"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
@@ -3402,15 +3447,15 @@
       <c r="C82" s="0"/>
       <c r="D82" s="0"/>
       <c r="E82" s="0"/>
-      <c r="F82" s="27"/>
+      <c r="F82" s="38"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="0"/>
-      <c r="F83" s="27"/>
+      <c r="F83" s="38"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
@@ -3418,15 +3463,15 @@
       <c r="C84" s="0"/>
       <c r="D84" s="0"/>
       <c r="E84" s="0"/>
-      <c r="F84" s="27"/>
+      <c r="F84" s="38"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
       <c r="E85" s="0"/>
-      <c r="F85" s="27"/>
+      <c r="F85" s="38"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
@@ -3434,15 +3479,15 @@
       <c r="C86" s="0"/>
       <c r="D86" s="0"/>
       <c r="E86" s="0"/>
-      <c r="F86" s="27"/>
+      <c r="F86" s="38"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
-      <c r="D87" s="34"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
       <c r="E87" s="0"/>
-      <c r="F87" s="27"/>
+      <c r="F87" s="38"/>
     </row>
     <row r="88" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
@@ -3450,15 +3495,15 @@
       <c r="C88" s="0"/>
       <c r="D88" s="0"/>
       <c r="E88" s="0"/>
-      <c r="F88" s="27"/>
+      <c r="F88" s="38"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
       <c r="E89" s="0"/>
-      <c r="F89" s="27"/>
+      <c r="F89" s="38"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
@@ -3466,15 +3511,15 @@
       <c r="C90" s="0"/>
       <c r="D90" s="0"/>
       <c r="E90" s="0"/>
-      <c r="F90" s="27"/>
+      <c r="F90" s="38"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
       <c r="E91" s="0"/>
-      <c r="F91" s="27"/>
+      <c r="F91" s="38"/>
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0"/>
@@ -3482,15 +3527,15 @@
       <c r="C92" s="0"/>
       <c r="D92" s="0"/>
       <c r="E92" s="0"/>
-      <c r="F92" s="27"/>
+      <c r="F92" s="38"/>
     </row>
     <row r="93" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
       <c r="E93" s="0"/>
-      <c r="F93" s="27"/>
+      <c r="F93" s="38"/>
     </row>
     <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
@@ -3498,15 +3543,15 @@
       <c r="C94" s="0"/>
       <c r="D94" s="0"/>
       <c r="E94" s="0"/>
-      <c r="F94" s="27"/>
+      <c r="F94" s="38"/>
     </row>
     <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="34"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
       <c r="E95" s="0"/>
-      <c r="F95" s="27"/>
+      <c r="F95" s="38"/>
     </row>
     <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
@@ -3514,15 +3559,15 @@
       <c r="C96" s="0"/>
       <c r="D96" s="0"/>
       <c r="E96" s="0"/>
-      <c r="F96" s="27"/>
+      <c r="F96" s="38"/>
     </row>
     <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="34"/>
-      <c r="D97" s="34"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
       <c r="E97" s="0"/>
-      <c r="F97" s="27"/>
+      <c r="F97" s="38"/>
     </row>
     <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
@@ -3530,15 +3575,15 @@
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
       <c r="E98" s="0"/>
-      <c r="F98" s="27"/>
+      <c r="F98" s="38"/>
     </row>
     <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
-      <c r="B99" s="34"/>
-      <c r="C99" s="34"/>
-      <c r="D99" s="34"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
       <c r="E99" s="0"/>
-      <c r="F99" s="27"/>
+      <c r="F99" s="38"/>
     </row>
     <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
@@ -3546,15 +3591,15 @@
       <c r="C100" s="0"/>
       <c r="D100" s="0"/>
       <c r="E100" s="0"/>
-      <c r="F100" s="27"/>
+      <c r="F100" s="38"/>
     </row>
     <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
-      <c r="B101" s="34"/>
-      <c r="C101" s="34"/>
-      <c r="D101" s="34"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
       <c r="E101" s="0"/>
-      <c r="F101" s="27"/>
+      <c r="F101" s="38"/>
     </row>
     <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
@@ -3562,15 +3607,15 @@
       <c r="C102" s="0"/>
       <c r="D102" s="0"/>
       <c r="E102" s="0"/>
-      <c r="F102" s="27"/>
+      <c r="F102" s="38"/>
     </row>
     <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
-      <c r="B103" s="34"/>
-      <c r="C103" s="34"/>
-      <c r="D103" s="34"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
       <c r="E103" s="0"/>
-      <c r="F103" s="27"/>
+      <c r="F103" s="38"/>
     </row>
     <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
@@ -3578,15 +3623,15 @@
       <c r="C104" s="0"/>
       <c r="D104" s="0"/>
       <c r="E104" s="0"/>
-      <c r="F104" s="27"/>
+      <c r="F104" s="38"/>
     </row>
     <row r="105" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0"/>
-      <c r="B105" s="34"/>
-      <c r="C105" s="34"/>
-      <c r="D105" s="34"/>
+      <c r="B105" s="39"/>
+      <c r="C105" s="39"/>
+      <c r="D105" s="39"/>
       <c r="E105" s="0"/>
-      <c r="F105" s="27"/>
+      <c r="F105" s="38"/>
     </row>
     <row r="106" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0"/>
@@ -3594,15 +3639,15 @@
       <c r="C106" s="0"/>
       <c r="D106" s="0"/>
       <c r="E106" s="0"/>
-      <c r="F106" s="27"/>
+      <c r="F106" s="38"/>
     </row>
     <row r="107" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0"/>
-      <c r="B107" s="34"/>
-      <c r="C107" s="34"/>
-      <c r="D107" s="34"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="39"/>
+      <c r="D107" s="39"/>
       <c r="E107" s="0"/>
-      <c r="F107" s="27"/>
+      <c r="F107" s="38"/>
     </row>
     <row r="108" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0"/>
@@ -3610,15 +3655,15 @@
       <c r="C108" s="0"/>
       <c r="D108" s="0"/>
       <c r="E108" s="0"/>
-      <c r="F108" s="27"/>
+      <c r="F108" s="38"/>
     </row>
     <row r="109" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0"/>
-      <c r="B109" s="34"/>
-      <c r="C109" s="34"/>
-      <c r="D109" s="34"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="39"/>
       <c r="E109" s="0"/>
-      <c r="F109" s="27"/>
+      <c r="F109" s="38"/>
     </row>
     <row r="110" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0"/>
@@ -3626,15 +3671,15 @@
       <c r="C110" s="0"/>
       <c r="D110" s="0"/>
       <c r="E110" s="0"/>
-      <c r="F110" s="27"/>
+      <c r="F110" s="38"/>
     </row>
     <row r="111" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0"/>
-      <c r="B111" s="34"/>
-      <c r="C111" s="34"/>
-      <c r="D111" s="34"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
       <c r="E111" s="0"/>
-      <c r="F111" s="27"/>
+      <c r="F111" s="38"/>
     </row>
     <row r="112" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0"/>
@@ -3642,206 +3687,206 @@
       <c r="C112" s="0"/>
       <c r="D112" s="0"/>
       <c r="E112" s="0"/>
-      <c r="F112" s="27"/>
+      <c r="F112" s="38"/>
     </row>
     <row r="113" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0"/>
-      <c r="B113" s="34"/>
-      <c r="C113" s="34"/>
-      <c r="D113" s="34"/>
+      <c r="B113" s="39"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
       <c r="E113" s="0"/>
-      <c r="F113" s="27"/>
+      <c r="F113" s="38"/>
     </row>
     <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
       <c r="B114" s="0"/>
       <c r="C114" s="0"/>
       <c r="D114" s="0"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
     </row>
     <row r="115" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
-      <c r="B115" s="34"/>
-      <c r="C115" s="34"/>
-      <c r="D115" s="34"/>
-      <c r="F115" s="27"/>
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="39"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="35"/>
-      <c r="B116" s="35"/>
-      <c r="C116" s="35"/>
-      <c r="D116" s="35"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="0"/>
-      <c r="F116" s="27"/>
+      <c r="F116" s="38"/>
     </row>
     <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="35"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
-      <c r="D117" s="35"/>
+      <c r="A117" s="40"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
+      <c r="D117" s="40"/>
       <c r="E117" s="0"/>
-      <c r="F117" s="27"/>
+      <c r="F117" s="38"/>
     </row>
     <row r="118" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="35"/>
-      <c r="B118" s="36"/>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
+      <c r="A118" s="40"/>
+      <c r="B118" s="41"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
       <c r="E118" s="0"/>
-      <c r="F118" s="27"/>
+      <c r="F118" s="38"/>
     </row>
     <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="35"/>
-      <c r="B119" s="35"/>
-      <c r="C119" s="35"/>
-      <c r="D119" s="35"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="0"/>
-      <c r="F119" s="27"/>
+      <c r="F119" s="38"/>
     </row>
     <row r="120" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="35"/>
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
+      <c r="A120" s="40"/>
+      <c r="B120" s="41"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
       <c r="E120" s="0"/>
-      <c r="F120" s="27"/>
+      <c r="F120" s="38"/>
     </row>
     <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="35"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
-      <c r="D121" s="35"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
-      <c r="F121" s="27"/>
+      <c r="F121" s="38"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="35"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
-      <c r="D122" s="35"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
       <c r="E122" s="0"/>
-      <c r="F122" s="27"/>
+      <c r="F122" s="38"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="35"/>
-      <c r="B123" s="36"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="41"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
       <c r="E123" s="0"/>
-      <c r="F123" s="27"/>
+      <c r="F123" s="38"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="35"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="35"/>
-      <c r="D124" s="35"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
       <c r="E124" s="0"/>
-      <c r="F124" s="27"/>
+      <c r="F124" s="38"/>
     </row>
     <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="35"/>
-      <c r="B125" s="36"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
+      <c r="A125" s="40"/>
+      <c r="B125" s="41"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="41"/>
       <c r="E125" s="0"/>
-      <c r="F125" s="27"/>
+      <c r="F125" s="38"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="35"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35"/>
-      <c r="D126" s="35"/>
+      <c r="A126" s="40"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
+      <c r="D126" s="40"/>
       <c r="E126" s="0"/>
-      <c r="F126" s="27"/>
+      <c r="F126" s="38"/>
     </row>
     <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="35"/>
-      <c r="B127" s="36"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="41"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
       <c r="E127" s="0"/>
-      <c r="F127" s="27"/>
+      <c r="F127" s="38"/>
     </row>
     <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="35"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="35"/>
-      <c r="D128" s="35"/>
+      <c r="A128" s="40"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
-      <c r="F128" s="27"/>
+      <c r="F128" s="38"/>
     </row>
     <row r="129" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="35"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="35"/>
-      <c r="D129" s="35"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="40"/>
+      <c r="C129" s="40"/>
+      <c r="D129" s="40"/>
       <c r="E129" s="0"/>
-      <c r="F129" s="27"/>
+      <c r="F129" s="38"/>
     </row>
     <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="35"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="35"/>
-      <c r="D130" s="35"/>
+      <c r="A130" s="40"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="40"/>
       <c r="E130" s="0"/>
-      <c r="F130" s="27"/>
+      <c r="F130" s="38"/>
     </row>
     <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="35"/>
-      <c r="B131" s="36"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="41"/>
+      <c r="C131" s="41"/>
+      <c r="D131" s="41"/>
       <c r="E131" s="0"/>
-      <c r="F131" s="27"/>
+      <c r="F131" s="38"/>
     </row>
     <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="35"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="35"/>
-      <c r="D132" s="35"/>
+      <c r="A132" s="40"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="40"/>
+      <c r="D132" s="40"/>
       <c r="E132" s="0"/>
-      <c r="F132" s="27"/>
+      <c r="F132" s="38"/>
     </row>
     <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="35"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="35"/>
-      <c r="D133" s="35"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="40"/>
+      <c r="D133" s="40"/>
       <c r="E133" s="0"/>
-      <c r="F133" s="27"/>
+      <c r="F133" s="38"/>
     </row>
     <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="35"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="35"/>
-      <c r="D134" s="35"/>
+      <c r="A134" s="40"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="40"/>
+      <c r="D134" s="40"/>
       <c r="E134" s="0"/>
-      <c r="F134" s="27"/>
+      <c r="F134" s="38"/>
     </row>
     <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="35"/>
-      <c r="B135" s="36"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="36"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="41"/>
+      <c r="C135" s="41"/>
+      <c r="D135" s="41"/>
       <c r="E135" s="0"/>
-      <c r="F135" s="27"/>
+      <c r="F135" s="38"/>
     </row>
     <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="35"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="35"/>
-      <c r="D136" s="35"/>
+      <c r="A136" s="40"/>
+      <c r="B136" s="40"/>
+      <c r="C136" s="40"/>
+      <c r="D136" s="40"/>
       <c r="E136" s="0"/>
-      <c r="F136" s="27"/>
+      <c r="F136" s="38"/>
     </row>
     <row r="137" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="35"/>
-      <c r="B137" s="36"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="36"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="41"/>
+      <c r="C137" s="41"/>
+      <c r="D137" s="41"/>
       <c r="E137" s="0"/>
-      <c r="F137" s="27"/>
+      <c r="F137" s="38"/>
     </row>
     <row r="138" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4120,12 +4165,12 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
@@ -4185,9 +4230,6 @@
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B137:D137"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" display="Note: corresponds to one of the realms defined at https://github.com/WCRP-CMIP/CMIP6_CVs/blob/master/CMIP6_realm.json."/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1. Address feedback to use descriptions exactly as given in CIM
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machine Performance</t>
   </si>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">Parallelisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or or all cores were used all of the time.</t>
+    <t xml:space="preserve">Total number of cores (NP) allocated for the run, regardless of whether or not all cores were used all of the time.</t>
   </si>
   <si>
     <t xml:space="preserve">Further detail: CPMIP Metrics: Coupling, memory and I/O</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Memory bloat</t>
   </si>
   <si>
-    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size to the ideal memory size (the size of the complete model state, which in theory is all you need to hold in memory)Mi, defined below.</t>
+    <t xml:space="preserve">Memory bloat is the ratio of the actual memory size, defined as M − NP × X where M is the measured runtime memory usage and X the size of the executable files, to the ideal memory size Mi, the size of the complete model state, which in theory is all you need to hold in memory.</t>
   </si>
   <si>
     <t xml:space="preserve">1.4.3</t>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">Data intensity</t>
   </si>
   <si>
-    <t xml:space="preserve">Data intensity the amount of data produced per compute-hour, in units GB per compute-hour.</t>
+    <t xml:space="preserve">Data intensity is the amount of data produced per compute-hour, in units GB per compute-hour.</t>
   </si>
   <si>
     <t xml:space="preserve">Performance of &lt;machine name&gt; for the &lt;realm name&gt; realm of model &lt;model name&gt;</t>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;realm name&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The energy cost of a simulation, measured in joules per simulated year (JPSY). Given the energy E in joules consumed over a budgeting interval T (generally 1 month or 1 year, in units of hours), JPSY=CHSY*E*T/NP</t>
   </si>
 </sst>
 </file>
@@ -810,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -947,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2608,7 +2605,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3196,7 +3193,7 @@
         <v>52</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>

</xml_diff>

<commit_message>
Address DH feedback RE performance spreadsheets template
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="101">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machine Performance</t>
   </si>
@@ -54,7 +54,7 @@
   </si>
   <si>
     <t xml:space="preserve">Important:
-For each tab, questions 1.1.5.1 and 1.1.5.2 ask if the performance outlined in the tab covers all applicable experiments or only some of them. In the latter case, where you wish to document groups of experiments or individual experiments separately from the others for a given combination of machine, model and realm (or aggregate across all realms), you should copy and then fill out the given tab as many times as required to provide performances to cover all of the possible applicable experiments with the desired partitioning.
+For each ‘Aggregate for’ tab (see below for details), questions 1.1.5.1 and 1.1.5.2 ask if the performance outlined in the tab covers all applicable experiments or only some of them. In the latter case, where you wish to document groups of experiments or individual experiments separately from the others for a given combination of machine, model and realm (or aggregate across all realms), you should copy and then fill out the given tab as many times as required to provide performances to cover all of the possible applicable experiments with the desired partitioning.
 For example, if for a given tab there are five listed experiments named A, B, C, D and E, you may document one performance covering all five experiments on one tab, OR copy the relevant tab five times and document one performance for all five separately, OR copy the tab two to four times to document the performance of some partitioning of experiments involving subsets of the overall five, for example one tab (and hence performance) for A and B, another tab for C and D, and a final one for E, or similar. Ensure that all experiments are included e.g. do not leave out any single one, such as E.</t>
   </si>
   <si>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">ALL</t>
   </si>
   <si>
-    <t xml:space="preserve">If you answered ‘ALL’ to the above, the following question (1.1.4.2) is not applicable so should be left blank, i.e. you are done for 1.1. Otherwise, please answer 1.1.4.2.</t>
+    <t xml:space="preserve">If you answered ‘ALL’ to the above, the following question (1.1.5.2) is not applicable so should be left blank, i.e. you are done for 1.1. Otherwise, please answer 1.1.5.2.</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.5.2</t>
@@ -862,7 +862,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -949,7 +949,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="399.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="460.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>9</v>
@@ -958,7 +958,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="621.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="589.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="12" t="s">
         <v>10</v>
@@ -1009,8 +1009,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="0"/>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
@@ -2758,8 +2758,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3022,7 +3022,7 @@
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="15.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0"/>
       <c r="C25" s="0"/>
@@ -3030,603 +3030,601 @@
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+    <row r="26" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="0"/>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="0"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="0"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="0"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
+      <c r="A29" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="0"/>
-      <c r="F29" s="28"/>
-    </row>
-    <row r="30" customFormat="false" ht="41.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="28"/>
+      <c r="F30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="32" t="n">
+        <v>1168884900</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
       <c r="E32" s="0"/>
-      <c r="F32" s="28"/>
-    </row>
-    <row r="33" customFormat="false" ht="160.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="0"/>
-      <c r="F33" s="28"/>
+      <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
+      <c r="A34" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="0"/>
       <c r="E34" s="0"/>
-      <c r="F34" s="28"/>
+      <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
-      <c r="D35" s="0"/>
+      <c r="B35" s="32" t="n">
+        <v>18</v>
+      </c>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="0"/>
-      <c r="F35" s="28"/>
-    </row>
-    <row r="36" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="F35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="0"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="0"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="0"/>
+      <c r="B39" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+    <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34"/>
-      <c r="B41" s="32" t="n">
-        <v>1168884900</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+    <row r="41" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
+      <c r="B42" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="C42" s="0"/>
-      <c r="D42" s="0"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="A43" s="0"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="0"/>
+      <c r="A44" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="32" t="n">
-        <v>18</v>
-      </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+      <c r="A45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="26"/>
+      <c r="D45" s="0"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="B46" s="36" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="0"/>
+      <c r="A48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="B49" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
+    <row r="49" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
+      <c r="B50" s="32" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
+    <row r="51" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="0"/>
-      <c r="D52" s="22"/>
+    <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
+    <row r="53" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="A54" s="0"/>
+      <c r="B54" s="32" t="n">
+        <v>585540</v>
+      </c>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="26"/>
+      <c r="A55" s="0"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="36" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
+      <c r="A56" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="D57" s="0"/>
+    <row r="57" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+      <c r="A58" s="0"/>
+      <c r="B58" s="38" t="n">
+        <v>23000000000</v>
+      </c>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
+    <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0"/>
-      <c r="B60" s="32" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
+    <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0"/>
-      <c r="B61" s="0"/>
-      <c r="C61" s="0"/>
+      <c r="A61" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="26"/>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
+      <c r="A62" s="0"/>
+      <c r="B62" s="36" t="n">
+        <v>12024</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
+    <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="32" t="n">
-        <v>585540</v>
-      </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
+    <row r="64" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="0"/>
-      <c r="F64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0"/>
-      <c r="B65" s="0"/>
-      <c r="C65" s="0"/>
-      <c r="D65" s="0"/>
+      <c r="F64" s="28"/>
+    </row>
+    <row r="65" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="35"/>
+      <c r="B65" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="0"/>
+      <c r="F65" s="28"/>
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="0"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25" t="s">
+      <c r="F66" s="28"/>
+    </row>
+    <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="28"/>
+    </row>
+    <row r="68" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B67" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="38" t="n">
-        <v>23000000000</v>
-      </c>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
+      <c r="B68" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
+      <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
-      <c r="D69" s="0"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
+      <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
+      <c r="A70" s="0"/>
+      <c r="B70" s="0"/>
+      <c r="C70" s="0"/>
+      <c r="D70" s="0"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="0"/>
+      <c r="F70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="0"/>
+      <c r="F71" s="28"/>
+    </row>
+    <row r="72" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="0"/>
-      <c r="E71" s="0"/>
-      <c r="F71" s="0"/>
-    </row>
-    <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0"/>
-      <c r="B72" s="36" t="n">
-        <v>12024</v>
-      </c>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
+      <c r="B72" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F72" s="28"/>
+    </row>
+    <row r="73" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
-      <c r="B73" s="0"/>
-      <c r="C73" s="0"/>
-      <c r="D73" s="0"/>
+      <c r="B73" s="36" t="n">
+        <v>183</v>
+      </c>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="0"/>
-    </row>
-    <row r="74" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="16" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
+      <c r="F73" s="28"/>
+    </row>
+    <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
+      <c r="D74" s="0"/>
       <c r="E74" s="0"/>
       <c r="F74" s="28"/>
     </row>
-    <row r="75" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="35"/>
-      <c r="B75" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
+    <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="0"/>
       <c r="F75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="25"/>
-      <c r="B76" s="26"/>
+      <c r="A76" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="C76" s="26"/>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
       <c r="F76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
+      <c r="A77" s="0"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
       <c r="E77" s="0"/>
       <c r="F77" s="28"/>
     </row>
-    <row r="78" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
+    <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
+      <c r="D78" s="0"/>
       <c r="E78" s="0"/>
       <c r="F78" s="28"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
+      <c r="A79" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="0"/>
       <c r="F79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0"/>
-      <c r="B80" s="0"/>
-      <c r="C80" s="0"/>
+      <c r="A80" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" s="26"/>
       <c r="D80" s="0"/>
       <c r="E80" s="0"/>
       <c r="F80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
+      <c r="A81" s="0"/>
+      <c r="B81" s="36" t="n">
+        <v>207</v>
+      </c>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
       <c r="E81" s="0"/>
       <c r="F81" s="28"/>
     </row>
-    <row r="82" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B82" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
+    <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
+      <c r="D82" s="0"/>
       <c r="E82" s="0"/>
       <c r="F82" s="28"/>
     </row>
-    <row r="83" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
-      <c r="B83" s="36" t="n">
-        <v>183</v>
-      </c>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="0"/>
       <c r="F83" s="28"/>
     </row>
@@ -3639,34 +3637,26 @@
       <c r="F84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
+      <c r="A85" s="0"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
       <c r="E85" s="0"/>
       <c r="F85" s="28"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="26"/>
+      <c r="A86" s="0"/>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
       <c r="D86" s="0"/>
       <c r="E86" s="0"/>
       <c r="F86" s="28"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
       <c r="E87" s="0"/>
       <c r="F87" s="28"/>
     </row>
@@ -3679,36 +3669,26 @@
       <c r="F88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
+      <c r="A89" s="0"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
       <c r="E89" s="0"/>
       <c r="F89" s="28"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B90" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" s="26"/>
+      <c r="A90" s="0"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
       <c r="D90" s="0"/>
       <c r="E90" s="0"/>
       <c r="F90" s="28"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
-      <c r="B91" s="36" t="n">
-        <v>207</v>
-      </c>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
       <c r="E91" s="0"/>
       <c r="F91" s="28"/>
     </row>
@@ -3736,7 +3716,7 @@
       <c r="E94" s="0"/>
       <c r="F94" s="28"/>
     </row>
-    <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -3744,7 +3724,7 @@
       <c r="E95" s="0"/>
       <c r="F95" s="28"/>
     </row>
-    <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -3752,7 +3732,7 @@
       <c r="E96" s="0"/>
       <c r="F96" s="28"/>
     </row>
-    <row r="97" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -3760,7 +3740,7 @@
       <c r="E97" s="0"/>
       <c r="F97" s="28"/>
     </row>
-    <row r="98" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
@@ -3768,7 +3748,7 @@
       <c r="E98" s="0"/>
       <c r="F98" s="28"/>
     </row>
-    <row r="99" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -3776,7 +3756,7 @@
       <c r="E99" s="0"/>
       <c r="F99" s="28"/>
     </row>
-    <row r="100" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
       <c r="B100" s="0"/>
       <c r="C100" s="0"/>
@@ -3784,7 +3764,7 @@
       <c r="E100" s="0"/>
       <c r="F100" s="28"/>
     </row>
-    <row r="101" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -3792,7 +3772,7 @@
       <c r="E101" s="0"/>
       <c r="F101" s="28"/>
     </row>
-    <row r="102" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
       <c r="B102" s="0"/>
       <c r="C102" s="0"/>
@@ -3800,7 +3780,7 @@
       <c r="E102" s="0"/>
       <c r="F102" s="28"/>
     </row>
-    <row r="103" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -3808,7 +3788,7 @@
       <c r="E103" s="0"/>
       <c r="F103" s="28"/>
     </row>
-    <row r="104" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
       <c r="B104" s="0"/>
       <c r="C104" s="0"/>
@@ -3893,94 +3873,94 @@
       <c r="B114" s="0"/>
       <c r="C114" s="0"/>
       <c r="D114" s="0"/>
-      <c r="E114" s="0"/>
+      <c r="E114" s="28"/>
       <c r="F114" s="28"/>
     </row>
-    <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
       <c r="D115" s="39"/>
-      <c r="E115" s="0"/>
       <c r="F115" s="28"/>
     </row>
     <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0"/>
-      <c r="B116" s="0"/>
-      <c r="C116" s="0"/>
-      <c r="D116" s="0"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="0"/>
       <c r="F116" s="28"/>
     </row>
-    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
+    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="40"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
+      <c r="D117" s="40"/>
       <c r="E117" s="0"/>
       <c r="F117" s="28"/>
     </row>
-    <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0"/>
-      <c r="B118" s="0"/>
-      <c r="C118" s="0"/>
-      <c r="D118" s="0"/>
+    <row r="118" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="40"/>
+      <c r="B118" s="41"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
       <c r="E118" s="0"/>
       <c r="F118" s="28"/>
     </row>
     <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="0"/>
       <c r="F119" s="28"/>
     </row>
-    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0"/>
-      <c r="B120" s="0"/>
-      <c r="C120" s="0"/>
-      <c r="D120" s="0"/>
+    <row r="120" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="40"/>
+      <c r="B120" s="41"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
       <c r="E120" s="0"/>
       <c r="F120" s="28"/>
     </row>
     <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0"/>
-      <c r="B122" s="0"/>
-      <c r="C122" s="0"/>
-      <c r="D122" s="0"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
       <c r="E122" s="0"/>
       <c r="F122" s="28"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="41"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
       <c r="E123" s="0"/>
       <c r="F123" s="28"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0"/>
-      <c r="B124" s="0"/>
-      <c r="C124" s="0"/>
-      <c r="D124" s="0"/>
-      <c r="E124" s="28"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
+      <c r="E124" s="0"/>
       <c r="F124" s="28"/>
     </row>
-    <row r="125" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0"/>
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
+    <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="40"/>
+      <c r="B125" s="41"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="41"/>
+      <c r="E125" s="0"/>
       <c r="F125" s="28"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3991,19 +3971,19 @@
       <c r="E126" s="0"/>
       <c r="F126" s="28"/>
     </row>
-    <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="40"/>
-      <c r="B127" s="40"/>
-      <c r="C127" s="40"/>
-      <c r="D127" s="40"/>
+      <c r="B127" s="41"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
       <c r="E127" s="0"/>
       <c r="F127" s="28"/>
     </row>
-    <row r="128" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="40"/>
-      <c r="B128" s="41"/>
-      <c r="C128" s="41"/>
-      <c r="D128" s="41"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
       <c r="F128" s="28"/>
     </row>
@@ -4015,23 +3995,23 @@
       <c r="E129" s="0"/>
       <c r="F129" s="28"/>
     </row>
-    <row r="130" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="40"/>
-      <c r="B130" s="41"/>
-      <c r="C130" s="41"/>
-      <c r="D130" s="41"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="40"/>
       <c r="E130" s="0"/>
       <c r="F130" s="28"/>
     </row>
-    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="40"/>
-      <c r="B131" s="40"/>
-      <c r="C131" s="40"/>
-      <c r="D131" s="40"/>
+      <c r="B131" s="41"/>
+      <c r="C131" s="41"/>
+      <c r="D131" s="41"/>
       <c r="E131" s="0"/>
       <c r="F131" s="28"/>
     </row>
-    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="40"/>
       <c r="B132" s="40"/>
       <c r="C132" s="40"/>
@@ -4039,11 +4019,11 @@
       <c r="E132" s="0"/>
       <c r="F132" s="28"/>
     </row>
-    <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="40"/>
-      <c r="B133" s="41"/>
-      <c r="C133" s="41"/>
-      <c r="D133" s="41"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="40"/>
+      <c r="D133" s="40"/>
       <c r="E133" s="0"/>
       <c r="F133" s="28"/>
     </row>
@@ -4055,7 +4035,7 @@
       <c r="E134" s="0"/>
       <c r="F134" s="28"/>
     </row>
-    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="40"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -4071,7 +4051,7 @@
       <c r="E136" s="0"/>
       <c r="F136" s="28"/>
     </row>
-    <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="40"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -4079,177 +4059,107 @@
       <c r="E137" s="0"/>
       <c r="F137" s="28"/>
     </row>
-    <row r="138" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="40"/>
-      <c r="B138" s="40"/>
-      <c r="C138" s="40"/>
-      <c r="D138" s="40"/>
-      <c r="E138" s="0"/>
-      <c r="F138" s="28"/>
-    </row>
-    <row r="139" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="40"/>
-      <c r="B139" s="40"/>
-      <c r="C139" s="40"/>
-      <c r="D139" s="40"/>
-      <c r="E139" s="0"/>
-      <c r="F139" s="28"/>
-    </row>
-    <row r="140" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="40"/>
-      <c r="B140" s="40"/>
-      <c r="C140" s="40"/>
-      <c r="D140" s="40"/>
-      <c r="E140" s="0"/>
-      <c r="F140" s="28"/>
-    </row>
-    <row r="141" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="40"/>
-      <c r="B141" s="41"/>
-      <c r="C141" s="41"/>
-      <c r="D141" s="41"/>
-      <c r="E141" s="0"/>
-      <c r="F141" s="28"/>
-    </row>
-    <row r="142" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="40"/>
-      <c r="B142" s="40"/>
-      <c r="C142" s="40"/>
-      <c r="D142" s="40"/>
-      <c r="E142" s="0"/>
-      <c r="F142" s="28"/>
-    </row>
-    <row r="143" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="40"/>
-      <c r="B143" s="40"/>
-      <c r="C143" s="40"/>
-      <c r="D143" s="40"/>
-      <c r="E143" s="0"/>
-      <c r="F143" s="28"/>
-    </row>
-    <row r="144" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="40"/>
-      <c r="B144" s="40"/>
-      <c r="C144" s="40"/>
-      <c r="D144" s="40"/>
-      <c r="E144" s="0"/>
-      <c r="F144" s="28"/>
-    </row>
-    <row r="145" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="40"/>
-      <c r="B145" s="41"/>
-      <c r="C145" s="41"/>
-      <c r="D145" s="41"/>
-      <c r="E145" s="0"/>
-      <c r="F145" s="28"/>
-    </row>
-    <row r="146" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="40"/>
-      <c r="B146" s="40"/>
-      <c r="C146" s="40"/>
-      <c r="D146" s="40"/>
-      <c r="E146" s="0"/>
-      <c r="F146" s="28"/>
-    </row>
-    <row r="147" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="40"/>
-      <c r="B147" s="41"/>
-      <c r="C147" s="41"/>
-      <c r="D147" s="41"/>
-      <c r="E147" s="0"/>
-      <c r="F147" s="28"/>
-    </row>
-    <row r="148" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="201" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="225" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="226" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="239" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="240" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="241" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4355,16 +4265,16 @@
     <row r="341" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="342" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4418,7 +4328,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="71">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
@@ -4432,41 +4342,39 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B67:D67"/>
     <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B71:D71"/>
     <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B73:D73"/>
     <mergeCell ref="B75:D75"/>
     <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B85:D85"/>
     <mergeCell ref="B87:D87"/>
@@ -4484,26 +4392,15 @@
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B113:D113"/>
     <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B120:D120"/>
     <mergeCell ref="B123:D123"/>
     <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B131:D131"/>
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B137:D137"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B145:D145"/>
-    <mergeCell ref="B147:D147"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B28" type="list">
-      <formula1>"ALL,SOME"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4521,8 +4418,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6264,7 +6161,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -6536,585 +6433,581 @@
       <c r="E25" s="0"/>
       <c r="F25" s="28"/>
     </row>
-    <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+    <row r="26" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="0"/>
       <c r="F26" s="28"/>
     </row>
-    <row r="27" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+    <row r="27" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="0"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="0"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="0"/>
       <c r="F28" s="28"/>
     </row>
     <row r="29" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
+      <c r="A29" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="0"/>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" customFormat="false" ht="41.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+    <row r="30" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="0"/>
       <c r="F30" s="28"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
       <c r="E32" s="0"/>
-      <c r="F32" s="28"/>
-    </row>
-    <row r="33" customFormat="false" ht="160.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="0"/>
-      <c r="F33" s="28"/>
+      <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
+      <c r="A34" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="0"/>
       <c r="E34" s="0"/>
-      <c r="F34" s="28"/>
-    </row>
-    <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
-      <c r="D35" s="0"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="0"/>
-      <c r="F35" s="28"/>
-    </row>
-    <row r="36" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="F35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
       <c r="E36" s="0"/>
-      <c r="F36" s="28"/>
-    </row>
-    <row r="37" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="0"/>
-      <c r="D37" s="22"/>
+      <c r="F36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="0"/>
-      <c r="F37" s="28"/>
+      <c r="F37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="0"/>
       <c r="E38" s="0"/>
-      <c r="F38" s="28"/>
+      <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="0"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
       <c r="E39" s="0"/>
-      <c r="F39" s="28"/>
-    </row>
-    <row r="40" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="F39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
       <c r="E40" s="0"/>
-      <c r="F40" s="28"/>
-    </row>
-    <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="F40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
+      <c r="B42" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="C42" s="0"/>
-      <c r="D42" s="0"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="A43" s="0"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="0"/>
+      <c r="A44" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+    <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="26"/>
+      <c r="D45" s="0"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="0"/>
+      <c r="A48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
+    <row r="49" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
+    <row r="51" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
-      <c r="B52" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="0"/>
-      <c r="D52" s="22"/>
+    <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
+    <row r="53" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="A54" s="0"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="26"/>
+      <c r="A55" s="0"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
+      <c r="A56" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="D57" s="0"/>
+    <row r="57" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+      <c r="A58" s="0"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
+    <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
+    <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0"/>
-      <c r="B61" s="0"/>
-      <c r="C61" s="0"/>
+      <c r="A61" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="26"/>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
+      <c r="A62" s="0"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
+    <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
+    <row r="64" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="0"/>
-      <c r="F64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0"/>
-      <c r="B65" s="0"/>
-      <c r="C65" s="0"/>
-      <c r="D65" s="0"/>
+      <c r="F64" s="28"/>
+    </row>
+    <row r="65" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="35"/>
+      <c r="B65" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="0"/>
-      <c r="F65" s="0"/>
+      <c r="F65" s="28"/>
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="0"/>
       <c r="E66" s="0"/>
-      <c r="F66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25" t="s">
+      <c r="F66" s="28"/>
+    </row>
+    <row r="67" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="0"/>
+      <c r="F67" s="28"/>
+    </row>
+    <row r="68" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B67" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
+      <c r="B68" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
+      <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
-      <c r="D69" s="0"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
       <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
+      <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
+      <c r="A70" s="0"/>
+      <c r="B70" s="0"/>
+      <c r="C70" s="0"/>
+      <c r="D70" s="0"/>
       <c r="E70" s="0"/>
-      <c r="F70" s="0"/>
+      <c r="F70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="0"/>
+      <c r="F71" s="28"/>
+    </row>
+    <row r="72" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="0"/>
-      <c r="E71" s="0"/>
-      <c r="F71" s="0"/>
-    </row>
-    <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
+      <c r="B72" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="0"/>
-      <c r="F72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F72" s="28"/>
+    </row>
+    <row r="73" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
-      <c r="B73" s="0"/>
-      <c r="C73" s="0"/>
-      <c r="D73" s="0"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
       <c r="E73" s="0"/>
-      <c r="F73" s="0"/>
-    </row>
-    <row r="74" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="16" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
+      <c r="F73" s="28"/>
+    </row>
+    <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
+      <c r="D74" s="0"/>
       <c r="E74" s="0"/>
       <c r="F74" s="28"/>
     </row>
-    <row r="75" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="35"/>
-      <c r="B75" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
+    <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="0"/>
       <c r="F75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="25"/>
-      <c r="B76" s="26"/>
+      <c r="A76" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="C76" s="26"/>
       <c r="D76" s="0"/>
       <c r="E76" s="0"/>
       <c r="F76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
+      <c r="A77" s="0"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
       <c r="E77" s="0"/>
       <c r="F77" s="28"/>
     </row>
-    <row r="78" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
+    <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
+      <c r="D78" s="0"/>
       <c r="E78" s="0"/>
       <c r="F78" s="28"/>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
+      <c r="A79" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="0"/>
       <c r="F79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0"/>
-      <c r="B80" s="0"/>
-      <c r="C80" s="0"/>
+      <c r="A80" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" s="26"/>
       <c r="D80" s="0"/>
       <c r="E80" s="0"/>
       <c r="F80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
+      <c r="A81" s="0"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
       <c r="E81" s="0"/>
       <c r="F81" s="28"/>
     </row>
-    <row r="82" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B82" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
+    <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
+      <c r="D82" s="0"/>
       <c r="E82" s="0"/>
       <c r="F82" s="28"/>
     </row>
-    <row r="83" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0"/>
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
       <c r="E83" s="0"/>
       <c r="F83" s="28"/>
     </row>
@@ -7127,34 +7020,26 @@
       <c r="F84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
+      <c r="A85" s="0"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
       <c r="E85" s="0"/>
       <c r="F85" s="28"/>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="26"/>
+      <c r="A86" s="0"/>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
       <c r="D86" s="0"/>
       <c r="E86" s="0"/>
       <c r="F86" s="28"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
       <c r="E87" s="0"/>
       <c r="F87" s="28"/>
     </row>
@@ -7167,34 +7052,26 @@
       <c r="F88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
+      <c r="A89" s="0"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
       <c r="E89" s="0"/>
       <c r="F89" s="28"/>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B90" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" s="26"/>
+      <c r="A90" s="0"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
       <c r="D90" s="0"/>
       <c r="E90" s="0"/>
       <c r="F90" s="28"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0"/>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
       <c r="E91" s="0"/>
       <c r="F91" s="28"/>
     </row>
@@ -7222,7 +7099,7 @@
       <c r="E94" s="0"/>
       <c r="F94" s="28"/>
     </row>
-    <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -7230,7 +7107,7 @@
       <c r="E95" s="0"/>
       <c r="F95" s="28"/>
     </row>
-    <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
@@ -7238,7 +7115,7 @@
       <c r="E96" s="0"/>
       <c r="F96" s="28"/>
     </row>
-    <row r="97" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -7246,7 +7123,7 @@
       <c r="E97" s="0"/>
       <c r="F97" s="28"/>
     </row>
-    <row r="98" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0"/>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
@@ -7254,7 +7131,7 @@
       <c r="E98" s="0"/>
       <c r="F98" s="28"/>
     </row>
-    <row r="99" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -7262,7 +7139,7 @@
       <c r="E99" s="0"/>
       <c r="F99" s="28"/>
     </row>
-    <row r="100" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
       <c r="B100" s="0"/>
       <c r="C100" s="0"/>
@@ -7270,7 +7147,7 @@
       <c r="E100" s="0"/>
       <c r="F100" s="28"/>
     </row>
-    <row r="101" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -7278,7 +7155,7 @@
       <c r="E101" s="0"/>
       <c r="F101" s="28"/>
     </row>
-    <row r="102" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0"/>
       <c r="B102" s="0"/>
       <c r="C102" s="0"/>
@@ -7286,7 +7163,7 @@
       <c r="E102" s="0"/>
       <c r="F102" s="28"/>
     </row>
-    <row r="103" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -7294,7 +7171,7 @@
       <c r="E103" s="0"/>
       <c r="F103" s="28"/>
     </row>
-    <row r="104" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
       <c r="B104" s="0"/>
       <c r="C104" s="0"/>
@@ -7379,94 +7256,94 @@
       <c r="B114" s="0"/>
       <c r="C114" s="0"/>
       <c r="D114" s="0"/>
-      <c r="E114" s="0"/>
+      <c r="E114" s="28"/>
       <c r="F114" s="28"/>
     </row>
-    <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
       <c r="D115" s="39"/>
-      <c r="E115" s="0"/>
       <c r="F115" s="28"/>
     </row>
     <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0"/>
-      <c r="B116" s="0"/>
-      <c r="C116" s="0"/>
-      <c r="D116" s="0"/>
+      <c r="A116" s="40"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="40"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="0"/>
       <c r="F116" s="28"/>
     </row>
-    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
+    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="40"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
+      <c r="D117" s="40"/>
       <c r="E117" s="0"/>
       <c r="F117" s="28"/>
     </row>
-    <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0"/>
-      <c r="B118" s="0"/>
-      <c r="C118" s="0"/>
-      <c r="D118" s="0"/>
+    <row r="118" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="40"/>
+      <c r="B118" s="41"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
       <c r="E118" s="0"/>
       <c r="F118" s="28"/>
     </row>
     <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="40"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="0"/>
       <c r="F119" s="28"/>
     </row>
-    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0"/>
-      <c r="B120" s="0"/>
-      <c r="C120" s="0"/>
-      <c r="D120" s="0"/>
+    <row r="120" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="40"/>
+      <c r="B120" s="41"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
       <c r="E120" s="0"/>
       <c r="F120" s="28"/>
     </row>
     <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0"/>
-      <c r="B122" s="0"/>
-      <c r="C122" s="0"/>
-      <c r="D122" s="0"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="40"/>
       <c r="E122" s="0"/>
       <c r="F122" s="28"/>
     </row>
     <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="41"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
       <c r="E123" s="0"/>
       <c r="F123" s="28"/>
     </row>
     <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0"/>
-      <c r="B124" s="0"/>
-      <c r="C124" s="0"/>
-      <c r="D124" s="0"/>
-      <c r="E124" s="28"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
+      <c r="E124" s="0"/>
       <c r="F124" s="28"/>
     </row>
-    <row r="125" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0"/>
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
+    <row r="125" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="40"/>
+      <c r="B125" s="41"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="41"/>
+      <c r="E125" s="0"/>
       <c r="F125" s="28"/>
     </row>
     <row r="126" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7477,19 +7354,19 @@
       <c r="E126" s="0"/>
       <c r="F126" s="28"/>
     </row>
-    <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="40"/>
-      <c r="B127" s="40"/>
-      <c r="C127" s="40"/>
-      <c r="D127" s="40"/>
+      <c r="B127" s="41"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
       <c r="E127" s="0"/>
       <c r="F127" s="28"/>
     </row>
-    <row r="128" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="40"/>
-      <c r="B128" s="41"/>
-      <c r="C128" s="41"/>
-      <c r="D128" s="41"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
       <c r="F128" s="28"/>
     </row>
@@ -7501,23 +7378,23 @@
       <c r="E129" s="0"/>
       <c r="F129" s="28"/>
     </row>
-    <row r="130" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="40"/>
-      <c r="B130" s="41"/>
-      <c r="C130" s="41"/>
-      <c r="D130" s="41"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
+      <c r="D130" s="40"/>
       <c r="E130" s="0"/>
       <c r="F130" s="28"/>
     </row>
-    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="40"/>
-      <c r="B131" s="40"/>
-      <c r="C131" s="40"/>
-      <c r="D131" s="40"/>
+      <c r="B131" s="41"/>
+      <c r="C131" s="41"/>
+      <c r="D131" s="41"/>
       <c r="E131" s="0"/>
       <c r="F131" s="28"/>
     </row>
-    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="40"/>
       <c r="B132" s="40"/>
       <c r="C132" s="40"/>
@@ -7525,11 +7402,11 @@
       <c r="E132" s="0"/>
       <c r="F132" s="28"/>
     </row>
-    <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="40"/>
-      <c r="B133" s="41"/>
-      <c r="C133" s="41"/>
-      <c r="D133" s="41"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="40"/>
+      <c r="D133" s="40"/>
       <c r="E133" s="0"/>
       <c r="F133" s="28"/>
     </row>
@@ -7541,7 +7418,7 @@
       <c r="E134" s="0"/>
       <c r="F134" s="28"/>
     </row>
-    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="40"/>
       <c r="B135" s="41"/>
       <c r="C135" s="41"/>
@@ -7557,7 +7434,7 @@
       <c r="E136" s="0"/>
       <c r="F136" s="28"/>
     </row>
-    <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="40"/>
       <c r="B137" s="41"/>
       <c r="C137" s="41"/>
@@ -7565,177 +7442,107 @@
       <c r="E137" s="0"/>
       <c r="F137" s="28"/>
     </row>
-    <row r="138" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="40"/>
-      <c r="B138" s="40"/>
-      <c r="C138" s="40"/>
-      <c r="D138" s="40"/>
-      <c r="E138" s="0"/>
-      <c r="F138" s="28"/>
-    </row>
-    <row r="139" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="40"/>
-      <c r="B139" s="40"/>
-      <c r="C139" s="40"/>
-      <c r="D139" s="40"/>
-      <c r="E139" s="0"/>
-      <c r="F139" s="28"/>
-    </row>
-    <row r="140" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="40"/>
-      <c r="B140" s="40"/>
-      <c r="C140" s="40"/>
-      <c r="D140" s="40"/>
-      <c r="E140" s="0"/>
-      <c r="F140" s="28"/>
-    </row>
-    <row r="141" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="40"/>
-      <c r="B141" s="41"/>
-      <c r="C141" s="41"/>
-      <c r="D141" s="41"/>
-      <c r="E141" s="0"/>
-      <c r="F141" s="28"/>
-    </row>
-    <row r="142" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="40"/>
-      <c r="B142" s="40"/>
-      <c r="C142" s="40"/>
-      <c r="D142" s="40"/>
-      <c r="E142" s="0"/>
-      <c r="F142" s="28"/>
-    </row>
-    <row r="143" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="40"/>
-      <c r="B143" s="40"/>
-      <c r="C143" s="40"/>
-      <c r="D143" s="40"/>
-      <c r="E143" s="0"/>
-      <c r="F143" s="28"/>
-    </row>
-    <row r="144" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="40"/>
-      <c r="B144" s="40"/>
-      <c r="C144" s="40"/>
-      <c r="D144" s="40"/>
-      <c r="E144" s="0"/>
-      <c r="F144" s="28"/>
-    </row>
-    <row r="145" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="40"/>
-      <c r="B145" s="41"/>
-      <c r="C145" s="41"/>
-      <c r="D145" s="41"/>
-      <c r="E145" s="0"/>
-      <c r="F145" s="28"/>
-    </row>
-    <row r="146" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="40"/>
-      <c r="B146" s="40"/>
-      <c r="C146" s="40"/>
-      <c r="D146" s="40"/>
-      <c r="E146" s="0"/>
-      <c r="F146" s="28"/>
-    </row>
-    <row r="147" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="40"/>
-      <c r="B147" s="41"/>
-      <c r="C147" s="41"/>
-      <c r="D147" s="41"/>
-      <c r="E147" s="0"/>
-      <c r="F147" s="28"/>
-    </row>
-    <row r="148" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="201" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="225" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="226" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="239" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="240" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="241" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7841,16 +7648,16 @@
     <row r="341" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="342" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7904,7 +7711,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="78">
+  <mergeCells count="71">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
@@ -7918,41 +7725,39 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B67:D67"/>
     <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B71:D71"/>
     <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B73:D73"/>
     <mergeCell ref="B75:D75"/>
     <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B85:D85"/>
     <mergeCell ref="B87:D87"/>
@@ -7970,26 +7775,15 @@
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B113:D113"/>
     <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B120:D120"/>
     <mergeCell ref="B123:D123"/>
     <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B131:D131"/>
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B137:D137"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B145:D145"/>
-    <mergeCell ref="B147:D147"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B28" type="list">
-      <formula1>"ALL,SOME"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update 'how to use' notes in performance template for new structure
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -59,7 +59,71 @@
     <t xml:space="preserve">https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO</t>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Please note the following:
+1. This spreadsheet covers a single machine and a single model only (both as named above). If your institute has multiple machines, you should have also received a separate set of spreadsheets for all other machines. For the given machine, you should have received a spreadsheet for every model applicable to the machine, the list of which was inferred from your </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">machines spreadsheet submission. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">If any of the models registered for this, or any other, machine are incorrect or missing in terms of spreadsheets received, please contact the ES-DOC team via </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">support@es-doc.org</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+2. For the machine and model in question, there are a set of tabs to complete: a top-level tab which covers the aggregate performance of the model across all of the modelling realms, plus a set of tabs which each cover the performance on a single one of the applicable realms of the model. The tab names and the pre-populated ‘Identity’ (item 1.1) values should clearly indicate the realm, or in the top-level tab case the aggregate across these, which each tab applies to for the given machine and model.
+3. For all tabs, please do not edit the pre-populated ‘Identity’ (item 1.1) values (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">except in the aggregate tab cases the question 1.1.5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> which have been greyed out in style to imply that they are not items to be completed as standard, rather that they are there to indicate the nature of the performance to be documented in each case (and also to verify the nature of each tab when the spreadsheet is parsed).</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Initialised by</t>
@@ -327,7 +391,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -381,6 +445,11 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -639,7 +708,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,43 +724,39 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,7 +764,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,39 +776,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -835,7 +904,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -932,7 +1001,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="397.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="563.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="12" t="s">
         <v>11</v>
@@ -966,6 +1035,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/"/>
+    <hyperlink ref="B10" r:id="rId2" display="support@es-doc.org"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>

</xml_diff>

<commit_message>
Address DH feedback by tweaking 'Applicable experiments' help text
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -59,71 +59,10 @@
     <t xml:space="preserve">https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Please note the following:
-1. This spreadsheet covers a single machine and a single model only (both as named above). If your institute has multiple machines, you should have also received a separate set of spreadsheets for all other machines. For the given machine, you should have received a spreadsheet for every model applicable to the machine, the list of which was inferred from your </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">machines spreadsheet submission. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">If any of the models registered for this, or any other, machine are incorrect or missing in terms of spreadsheets received, please contact the ES-DOC team via </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">support@es-doc.org</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.
+    <t xml:space="preserve">Please note the following:
+1. This spreadsheet covers a single machine and a single model only (both as named above). If your institute has multiple machines, you should have also received a separate set of spreadsheets for all other machines. For the given machine, you should have received a spreadsheet for every model applicable to the machine, the list of which was inferred from your machines spreadsheet submission. If any of the models registered for this, or any other, machine are incorrect or missing in terms of spreadsheets received, please contact the ES-DOC team via support@es-doc.org.
 2. For the machine and model in question, there are a set of tabs to complete: a top-level tab which covers the aggregate performance of the model across all of the modelling realms, plus a set of tabs which each cover the performance on a single one of the applicable realms of the model. The tab names and the pre-populated ‘Identity’ (item 1.1) values should clearly indicate the realm, or in the top-level tab case the aggregate across these, which each tab applies to for the given machine and model.
-3. For all tabs, please do not edit the pre-populated ‘Identity’ (item 1.1) values (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">except in the aggregate tab cases the question 1.1.5)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> which have been greyed out in style to imply that they are not items to be completed as standard, rather that they are there to indicate the nature of the performance to be documented in each case (and also to verify the nature of each tab when the spreadsheet is parsed).</t>
-    </r>
+3. For all tabs, please do not edit the pre-populated ‘Identity’ (item 1.1) values (except in the aggregate tab cases the question 1.1.5) which have been greyed out in style to imply that they are not items to be completed as standard, rather that they are there to indicate the nature of the performance to be documented in each case (and also to verify the nature of each tab when the spreadsheet is parsed).</t>
   </si>
   <si>
     <t xml:space="preserve">Initialised by</t>
@@ -207,7 +146,7 @@
     <t xml:space="preserve">ENUM</t>
   </si>
   <si>
-    <t xml:space="preserve">Which experiment(s) does this performance apply to: list all of the experiments which this performance applies to, where the list of potential choices is the list of all experiments for CMIP6 and the pre-populated answers, which may be edited, are drawn from the answers you provided to the ‘applicable experiments by MIP’ questions in the spreadsheet you submitted for this machine?
+    <t xml:space="preserve">Which experiment(s) does this performance apply to: list all of the experiments to which this performance applies, where the list of potential choices is the list of all experiments for CMIP6 and the pre-populated answers, which may be edited, are drawn from the answers you provided to the ‘applicable experiments by MIP’ questions in the spreadsheet you submitted for this machine.
 Select the experiment(s) from the enumerated list below on a case-by-case basis, by entering a new (input box) row, copying &amp; pasting an existing row, and editing accordingly should you need to list multiple cases.</t>
   </si>
   <si>
@@ -391,7 +330,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -445,11 +384,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -724,39 +658,43 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -764,11 +702,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -776,39 +710,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,8 +837,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1035,7 +969,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://es-doc.org/how-to-use-institute-machine-performance-spreadsheets/"/>
-    <hyperlink ref="B10" r:id="rId2" display="support@es-doc.org"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -1054,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4388,7 +4321,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Address DH feedback by addding greyed-out item 1.1.5 to realm tabs
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="99">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machine Performance for a given Model</t>
   </si>
@@ -297,6 +297,9 @@
     <t xml:space="preserve">ocean</t>
   </si>
   <si>
+    <t xml:space="preserve">Not applicable, applies to all experiments specified by the aggregate performance for HadGEM3-GC3.1 N512 ORCA12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aggregate (across all realms) performance of &lt;machine name&gt; for model &lt;model name&gt;</t>
   </si>
   <si>
@@ -319,6 +322,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;realm name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not applicable, applies to all experiments specified by the aggregate performance for &lt;model name&gt;</t>
   </si>
 </sst>
 </file>
@@ -987,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2667,8 +2673,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2931,106 +2937,106 @@
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+    <row r="25" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="0"/>
-      <c r="D26" s="22"/>
+    <row r="26" customFormat="false" ht="113.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="22"/>
+      <c r="B27" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="0"/>
       <c r="F27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+    <row r="28" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="A29" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="0"/>
       <c r="F29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="33"/>
-      <c r="B30" s="32" t="n">
-        <v>1168884900</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+      <c r="A30" s="0"/>
+      <c r="B30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="0"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="0"/>
       <c r="F30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="45.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="0"/>
+      <c r="B33" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="32" t="n">
-        <v>18</v>
+        <v>1168884900</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
@@ -3047,10 +3053,10 @@
     </row>
     <row r="36" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
@@ -3058,11 +3064,11 @@
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="34" t="s">
-        <v>21</v>
+      <c r="A37" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="0"/>
@@ -3071,11 +3077,11 @@
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
-      <c r="B38" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
+      <c r="B38" s="32" t="n">
+        <v>18</v>
+      </c>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
@@ -3087,109 +3093,109 @@
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+    <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="0"/>
-      <c r="D41" s="22"/>
+    <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="0"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
+      <c r="B42" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="0"/>
+    <row r="44" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
-      <c r="B45" s="35" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
+      <c r="B45" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="0"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
+      <c r="B48" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="0"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
-      <c r="B49" s="32" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
+      <c r="B49" s="35" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
@@ -3203,32 +3209,32 @@
     </row>
     <row r="51" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="31"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="32" t="n">
-        <v>585540</v>
+        <v>0.34</v>
       </c>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
@@ -3245,22 +3251,22 @@
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
@@ -3269,11 +3275,11 @@
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
-      <c r="B57" s="37" t="n">
-        <v>23000000000</v>
-      </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="32" t="n">
+        <v>585540</v>
+      </c>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
@@ -3287,35 +3293,35 @@
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="0"/>
+      <c r="B60" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
-      <c r="B61" s="35" t="n">
-        <v>12024</v>
-      </c>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
+      <c r="B61" s="37" t="n">
+        <v>23000000000</v>
+      </c>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
@@ -3327,105 +3333,105 @@
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="n">
+    <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="26"/>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="35" t="n">
+        <v>12024</v>
+      </c>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="0"/>
+      <c r="F65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
+      <c r="F66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="n">
         <v>1.4</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B67" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="0"/>
-      <c r="F63" s="28"/>
-    </row>
-    <row r="64" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="34"/>
-      <c r="B64" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="0"/>
-      <c r="F64" s="28"/>
-    </row>
-    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="25"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="0"/>
-      <c r="E65" s="0"/>
-      <c r="F65" s="28"/>
-    </row>
-    <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="0"/>
-      <c r="F66" s="28"/>
-    </row>
-    <row r="67" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
       <c r="E67" s="0"/>
       <c r="F67" s="28"/>
     </row>
-    <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
+    <row r="68" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="34"/>
+      <c r="B68" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
       <c r="E68" s="0"/>
       <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="0"/>
       <c r="E69" s="0"/>
       <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="30"/>
       <c r="E70" s="0"/>
       <c r="F70" s="28"/>
     </row>
-    <row r="71" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="0"/>
       <c r="F71" s="28"/>
     </row>
-    <row r="72" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
-      <c r="B72" s="35" t="n">
-        <v>183</v>
-      </c>
+      <c r="B72" s="35"/>
       <c r="C72" s="35"/>
       <c r="D72" s="35"/>
       <c r="E72" s="0"/>
@@ -3441,31 +3447,33 @@
     </row>
     <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="30"/>
       <c r="E74" s="0"/>
       <c r="F74" s="28"/>
     </row>
-    <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="26"/>
-      <c r="D75" s="0"/>
+      <c r="B75" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
       <c r="E75" s="0"/>
       <c r="F75" s="28"/>
     </row>
-    <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0"/>
-      <c r="B76" s="35"/>
+      <c r="B76" s="35" t="n">
+        <v>183</v>
+      </c>
       <c r="C76" s="35"/>
       <c r="D76" s="35"/>
       <c r="E76" s="0"/>
@@ -3481,10 +3489,10 @@
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C78" s="30"/>
       <c r="D78" s="30"/>
@@ -3496,7 +3504,7 @@
         <v>58</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="0"/>
@@ -3505,9 +3513,7 @@
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0"/>
-      <c r="B80" s="35" t="n">
-        <v>207</v>
-      </c>
+      <c r="B80" s="35"/>
       <c r="C80" s="35"/>
       <c r="D80" s="35"/>
       <c r="E80" s="0"/>
@@ -3522,26 +3528,36 @@
       <c r="F81" s="28"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
+      <c r="A82" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="0"/>
       <c r="F82" s="28"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0"/>
-      <c r="B83" s="0"/>
-      <c r="C83" s="0"/>
+      <c r="A83" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="26"/>
       <c r="D83" s="0"/>
       <c r="E83" s="0"/>
       <c r="F83" s="28"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
+      <c r="B84" s="35" t="n">
+        <v>207</v>
+      </c>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="0"/>
       <c r="F84" s="28"/>
     </row>
@@ -3617,7 +3633,7 @@
       <c r="E93" s="0"/>
       <c r="F93" s="28"/>
     </row>
-    <row r="94" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
       <c r="B94" s="38"/>
       <c r="C94" s="38"/>
@@ -3625,7 +3641,7 @@
       <c r="E94" s="0"/>
       <c r="F94" s="28"/>
     </row>
-    <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -3633,7 +3649,7 @@
       <c r="E95" s="0"/>
       <c r="F95" s="28"/>
     </row>
-    <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
       <c r="B96" s="38"/>
       <c r="C96" s="38"/>
@@ -3641,7 +3657,7 @@
       <c r="E96" s="0"/>
       <c r="F96" s="28"/>
     </row>
-    <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
@@ -3774,57 +3790,57 @@
       <c r="B113" s="0"/>
       <c r="C113" s="0"/>
       <c r="D113" s="0"/>
-      <c r="E113" s="28"/>
+      <c r="E113" s="0"/>
       <c r="F113" s="28"/>
     </row>
-    <row r="114" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
       <c r="B114" s="38"/>
       <c r="C114" s="38"/>
       <c r="D114" s="38"/>
+      <c r="E114" s="0"/>
       <c r="F114" s="28"/>
     </row>
     <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="39"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
+      <c r="A115" s="0"/>
+      <c r="B115" s="0"/>
+      <c r="C115" s="0"/>
+      <c r="D115" s="0"/>
       <c r="E115" s="0"/>
       <c r="F115" s="28"/>
     </row>
-    <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="39"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
+    <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
       <c r="E116" s="0"/>
       <c r="F116" s="28"/>
     </row>
-    <row r="117" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="39"/>
-      <c r="B117" s="40"/>
-      <c r="C117" s="40"/>
-      <c r="D117" s="40"/>
-      <c r="E117" s="0"/>
+    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0"/>
+      <c r="B117" s="0"/>
+      <c r="C117" s="0"/>
+      <c r="D117" s="0"/>
+      <c r="E117" s="28"/>
       <c r="F117" s="28"/>
     </row>
-    <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="39"/>
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="0"/>
+    <row r="118" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
       <c r="F118" s="28"/>
     </row>
-    <row r="119" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="39"/>
-      <c r="B119" s="40"/>
-      <c r="C119" s="40"/>
-      <c r="D119" s="40"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
       <c r="E119" s="0"/>
       <c r="F119" s="28"/>
     </row>
-    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -3832,35 +3848,35 @@
       <c r="E120" s="0"/>
       <c r="F120" s="28"/>
     </row>
-    <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="39"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="39"/>
-      <c r="B122" s="40"/>
-      <c r="C122" s="40"/>
-      <c r="D122" s="40"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
       <c r="E122" s="0"/>
       <c r="F122" s="28"/>
     </row>
-    <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="39"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="40"/>
       <c r="E123" s="0"/>
       <c r="F123" s="28"/>
     </row>
-    <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="39"/>
-      <c r="B124" s="40"/>
-      <c r="C124" s="40"/>
-      <c r="D124" s="40"/>
+      <c r="B124" s="39"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="39"/>
       <c r="E124" s="0"/>
       <c r="F124" s="28"/>
     </row>
@@ -3888,11 +3904,11 @@
       <c r="E127" s="0"/>
       <c r="F127" s="28"/>
     </row>
-    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="39"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="39"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
       <c r="F128" s="28"/>
     </row>
@@ -3904,7 +3920,7 @@
       <c r="E129" s="0"/>
       <c r="F129" s="28"/>
     </row>
-    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="39"/>
       <c r="B130" s="40"/>
       <c r="C130" s="40"/>
@@ -3912,7 +3928,7 @@
       <c r="E130" s="0"/>
       <c r="F130" s="28"/>
     </row>
-    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -3920,7 +3936,7 @@
       <c r="E131" s="0"/>
       <c r="F131" s="28"/>
     </row>
-    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -3936,7 +3952,7 @@
       <c r="E133" s="0"/>
       <c r="F133" s="28"/>
     </row>
-    <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="39"/>
       <c r="B134" s="40"/>
       <c r="C134" s="40"/>
@@ -3944,7 +3960,7 @@
       <c r="E134" s="0"/>
       <c r="F134" s="28"/>
     </row>
-    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -3952,64 +3968,92 @@
       <c r="E135" s="0"/>
       <c r="F135" s="28"/>
     </row>
-    <row r="136" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="39"/>
-      <c r="B136" s="40"/>
-      <c r="C136" s="40"/>
-      <c r="D136" s="40"/>
+      <c r="B136" s="39"/>
+      <c r="C136" s="39"/>
+      <c r="D136" s="39"/>
       <c r="E136" s="0"/>
       <c r="F136" s="28"/>
     </row>
-    <row r="137" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="39"/>
+      <c r="B137" s="39"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="0"/>
+      <c r="F137" s="28"/>
+    </row>
+    <row r="138" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="39"/>
+      <c r="B138" s="40"/>
+      <c r="C138" s="40"/>
+      <c r="D138" s="40"/>
+      <c r="E138" s="0"/>
+      <c r="F138" s="28"/>
+    </row>
+    <row r="139" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="39"/>
+      <c r="B139" s="39"/>
+      <c r="C139" s="39"/>
+      <c r="D139" s="39"/>
+      <c r="E139" s="0"/>
+      <c r="F139" s="28"/>
+    </row>
+    <row r="140" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A140" s="39"/>
+      <c r="B140" s="40"/>
+      <c r="C140" s="40"/>
+      <c r="D140" s="40"/>
+      <c r="E140" s="0"/>
+      <c r="F140" s="28"/>
+    </row>
+    <row r="141" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4017,44 +4061,44 @@
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="211" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="218" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="219" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="221" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="223" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="224" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="225" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="233" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="234" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4166,10 +4210,10 @@
     <row r="340" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="341" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="342" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4230,7 +4274,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="71">
+  <mergeCells count="74">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -4244,18 +4288,18 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B51:D51"/>
     <mergeCell ref="B52:D52"/>
@@ -4264,16 +4308,17 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:D61"/>
     <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B67:D67"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B78:D78"/>
     <mergeCell ref="B80:D80"/>
@@ -4294,14 +4339,16 @@
     <mergeCell ref="B110:D110"/>
     <mergeCell ref="B112:D112"/>
     <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="B123:D123"/>
     <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B128:D128"/>
     <mergeCell ref="B130:D130"/>
     <mergeCell ref="B134:D134"/>
-    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B140:D140"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
@@ -4321,7 +4368,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4341,7 +4388,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -4425,7 +4472,7 @@
     <row r="9" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
@@ -4467,7 +4514,7 @@
     <row r="13" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
@@ -4509,7 +4556,7 @@
     <row r="17" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -4611,7 +4658,7 @@
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C27" s="32"/>
       <c r="D27" s="32"/>
@@ -5995,7 +6042,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6015,7 +6062,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -6099,7 +6146,7 @@
     <row r="9" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
@@ -6141,7 +6188,7 @@
     <row r="13" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
@@ -6183,7 +6230,7 @@
     <row r="17" customFormat="false" ht="23.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -6243,7 +6290,7 @@
     <row r="23" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
@@ -6258,102 +6305,104 @@
       <c r="E24" s="0"/>
       <c r="F24" s="28"/>
     </row>
-    <row r="25" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+    <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="0"/>
       <c r="F25" s="28"/>
     </row>
-    <row r="26" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="0"/>
-      <c r="D26" s="22"/>
+    <row r="26" customFormat="false" ht="115.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="0"/>
       <c r="F26" s="28"/>
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="22"/>
+      <c r="B27" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="0"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
       <c r="E28" s="0"/>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+    <row r="29" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="0"/>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="33"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
+    <row r="30" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="0"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F32" s="28"/>
+    </row>
+    <row r="33" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="0"/>
+      <c r="B33" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
+      <c r="F33" s="28"/>
+    </row>
+    <row r="34" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="33"/>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
@@ -6370,10 +6419,10 @@
     </row>
     <row r="36" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
@@ -6381,22 +6430,22 @@
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="34" t="s">
-        <v>21</v>
+      <c r="A37" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="0"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="0"/>
       <c r="F38" s="0"/>
     </row>
@@ -6408,105 +6457,105 @@
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+    <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="0"/>
-      <c r="D41" s="22"/>
+    <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="0"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
       <c r="E43" s="0"/>
       <c r="F43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="0"/>
+    <row r="44" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
+      <c r="B45" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="0"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="0"/>
       <c r="F45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
       <c r="E46" s="0"/>
       <c r="F46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
       <c r="E47" s="0"/>
       <c r="F47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
+      <c r="B48" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="0"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
       <c r="E49" s="0"/>
       <c r="F49" s="0"/>
     </row>
@@ -6520,29 +6569,29 @@
     </row>
     <row r="51" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C52" s="31"/>
       <c r="D52" s="31"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
@@ -6560,22 +6609,22 @@
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="53.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
@@ -6584,9 +6633,9 @@
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
@@ -6600,33 +6649,33 @@
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="39.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="0"/>
+      <c r="B60" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
     </row>
@@ -6638,101 +6687,101 @@
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="n">
+    <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="26"/>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="0"/>
+      <c r="F65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
+      <c r="F66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="52.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="n">
         <v>1.4</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B67" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="0"/>
-      <c r="F63" s="28"/>
-    </row>
-    <row r="64" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="34"/>
-      <c r="B64" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="0"/>
-      <c r="F64" s="28"/>
-    </row>
-    <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="25"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="0"/>
-      <c r="E65" s="0"/>
-      <c r="F65" s="28"/>
-    </row>
-    <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="0"/>
-      <c r="F66" s="28"/>
-    </row>
-    <row r="67" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
       <c r="E67" s="0"/>
       <c r="F67" s="28"/>
     </row>
-    <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
+    <row r="68" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="34"/>
+      <c r="B68" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
       <c r="E68" s="0"/>
       <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0"/>
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="0"/>
       <c r="E69" s="0"/>
       <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="30"/>
       <c r="E70" s="0"/>
       <c r="F70" s="28"/>
     </row>
-    <row r="71" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="67.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="0"/>
       <c r="F71" s="28"/>
     </row>
-    <row r="72" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="35"/>
       <c r="C72" s="35"/>
@@ -6750,29 +6799,29 @@
     </row>
     <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="30"/>
       <c r="E74" s="0"/>
       <c r="F74" s="28"/>
     </row>
-    <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="26"/>
-      <c r="D75" s="0"/>
+      <c r="B75" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
       <c r="E75" s="0"/>
       <c r="F75" s="28"/>
     </row>
-    <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0"/>
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
@@ -6790,10 +6839,10 @@
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C78" s="30"/>
       <c r="D78" s="30"/>
@@ -6805,7 +6854,7 @@
         <v>58</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C79" s="26"/>
       <c r="D79" s="0"/>
@@ -6829,26 +6878,34 @@
       <c r="F81" s="28"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
+      <c r="A82" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="0"/>
       <c r="F82" s="28"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0"/>
-      <c r="B83" s="0"/>
-      <c r="C83" s="0"/>
+      <c r="A83" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="26"/>
       <c r="D83" s="0"/>
       <c r="E83" s="0"/>
       <c r="F83" s="28"/>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="0"/>
       <c r="F84" s="28"/>
     </row>
@@ -6924,7 +6981,7 @@
       <c r="E93" s="0"/>
       <c r="F93" s="28"/>
     </row>
-    <row r="94" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
       <c r="B94" s="38"/>
       <c r="C94" s="38"/>
@@ -6932,7 +6989,7 @@
       <c r="E94" s="0"/>
       <c r="F94" s="28"/>
     </row>
-    <row r="95" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
@@ -6940,7 +6997,7 @@
       <c r="E95" s="0"/>
       <c r="F95" s="28"/>
     </row>
-    <row r="96" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
       <c r="B96" s="38"/>
       <c r="C96" s="38"/>
@@ -6948,7 +7005,7 @@
       <c r="E96" s="0"/>
       <c r="F96" s="28"/>
     </row>
-    <row r="97" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
@@ -7081,57 +7138,57 @@
       <c r="B113" s="0"/>
       <c r="C113" s="0"/>
       <c r="D113" s="0"/>
-      <c r="E113" s="28"/>
+      <c r="E113" s="0"/>
       <c r="F113" s="28"/>
     </row>
-    <row r="114" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
       <c r="B114" s="38"/>
       <c r="C114" s="38"/>
       <c r="D114" s="38"/>
+      <c r="E114" s="0"/>
       <c r="F114" s="28"/>
     </row>
     <row r="115" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="39"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
+      <c r="A115" s="0"/>
+      <c r="B115" s="0"/>
+      <c r="C115" s="0"/>
+      <c r="D115" s="0"/>
       <c r="E115" s="0"/>
       <c r="F115" s="28"/>
     </row>
-    <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="39"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
+    <row r="116" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
       <c r="E116" s="0"/>
       <c r="F116" s="28"/>
     </row>
-    <row r="117" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="39"/>
-      <c r="B117" s="40"/>
-      <c r="C117" s="40"/>
-      <c r="D117" s="40"/>
-      <c r="E117" s="0"/>
+    <row r="117" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0"/>
+      <c r="B117" s="0"/>
+      <c r="C117" s="0"/>
+      <c r="D117" s="0"/>
+      <c r="E117" s="28"/>
       <c r="F117" s="28"/>
     </row>
-    <row r="118" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="39"/>
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="0"/>
+    <row r="118" customFormat="false" ht="47.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
       <c r="F118" s="28"/>
     </row>
-    <row r="119" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="39"/>
-      <c r="B119" s="40"/>
-      <c r="C119" s="40"/>
-      <c r="D119" s="40"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
       <c r="E119" s="0"/>
       <c r="F119" s="28"/>
     </row>
-    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -7139,35 +7196,35 @@
       <c r="E120" s="0"/>
       <c r="F120" s="28"/>
     </row>
-    <row r="121" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="39"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="0"/>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="39"/>
-      <c r="B122" s="40"/>
-      <c r="C122" s="40"/>
-      <c r="D122" s="40"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
       <c r="E122" s="0"/>
       <c r="F122" s="28"/>
     </row>
-    <row r="123" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="39"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="40"/>
       <c r="E123" s="0"/>
       <c r="F123" s="28"/>
     </row>
-    <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="39"/>
-      <c r="B124" s="40"/>
-      <c r="C124" s="40"/>
-      <c r="D124" s="40"/>
+      <c r="B124" s="39"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="39"/>
       <c r="E124" s="0"/>
       <c r="F124" s="28"/>
     </row>
@@ -7195,11 +7252,11 @@
       <c r="E127" s="0"/>
       <c r="F127" s="28"/>
     </row>
-    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="39"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="39"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="0"/>
       <c r="F128" s="28"/>
     </row>
@@ -7211,7 +7268,7 @@
       <c r="E129" s="0"/>
       <c r="F129" s="28"/>
     </row>
-    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="39"/>
       <c r="B130" s="40"/>
       <c r="C130" s="40"/>
@@ -7219,7 +7276,7 @@
       <c r="E130" s="0"/>
       <c r="F130" s="28"/>
     </row>
-    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -7227,7 +7284,7 @@
       <c r="E131" s="0"/>
       <c r="F131" s="28"/>
     </row>
-    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -7243,7 +7300,7 @@
       <c r="E133" s="0"/>
       <c r="F133" s="28"/>
     </row>
-    <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="39"/>
       <c r="B134" s="40"/>
       <c r="C134" s="40"/>
@@ -7251,7 +7308,7 @@
       <c r="E134" s="0"/>
       <c r="F134" s="28"/>
     </row>
-    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -7259,64 +7316,92 @@
       <c r="E135" s="0"/>
       <c r="F135" s="28"/>
     </row>
-    <row r="136" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="39"/>
-      <c r="B136" s="40"/>
-      <c r="C136" s="40"/>
-      <c r="D136" s="40"/>
+      <c r="B136" s="39"/>
+      <c r="C136" s="39"/>
+      <c r="D136" s="39"/>
       <c r="E136" s="0"/>
       <c r="F136" s="28"/>
     </row>
-    <row r="137" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="39"/>
+      <c r="B137" s="39"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="0"/>
+      <c r="F137" s="28"/>
+    </row>
+    <row r="138" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="39"/>
+      <c r="B138" s="40"/>
+      <c r="C138" s="40"/>
+      <c r="D138" s="40"/>
+      <c r="E138" s="0"/>
+      <c r="F138" s="28"/>
+    </row>
+    <row r="139" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="39"/>
+      <c r="B139" s="39"/>
+      <c r="C139" s="39"/>
+      <c r="D139" s="39"/>
+      <c r="E139" s="0"/>
+      <c r="F139" s="28"/>
+    </row>
+    <row r="140" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A140" s="39"/>
+      <c r="B140" s="40"/>
+      <c r="C140" s="40"/>
+      <c r="D140" s="40"/>
+      <c r="E140" s="0"/>
+      <c r="F140" s="28"/>
+    </row>
+    <row r="141" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="114.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="43.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7324,44 +7409,44 @@
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="151.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="211" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="218" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="219" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="221" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="223" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="224" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="225" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="233" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="234" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7473,10 +7558,10 @@
     <row r="340" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="341" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="342" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7537,7 +7622,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="71">
+  <mergeCells count="74">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -7551,18 +7636,18 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B51:D51"/>
     <mergeCell ref="B52:D52"/>
@@ -7571,16 +7656,17 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:D61"/>
     <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B67:D67"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B78:D78"/>
     <mergeCell ref="B80:D80"/>
@@ -7601,14 +7687,16 @@
     <mergeCell ref="B110:D110"/>
     <mergeCell ref="B112:D112"/>
     <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B121:D121"/>
+    <mergeCell ref="B123:D123"/>
     <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B128:D128"/>
     <mergeCell ref="B130:D130"/>
     <mergeCell ref="B134:D134"/>
-    <mergeCell ref="B136:D136"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B140:D140"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>

</xml_diff>

<commit_message>
Remove 'not applicable' from help text as it may confuse
</commit_message>
<xml_diff>
--- a/lib/machines/templates/performance.xlsx
+++ b/lib/machines/templates/performance.xlsx
@@ -297,7 +297,7 @@
     <t xml:space="preserve">ocean</t>
   </si>
   <si>
-    <t xml:space="preserve">Not applicable, applies to all experiments specified by the aggregate performance for HadGEM3-GC3.1 N512 ORCA12</t>
+    <t xml:space="preserve">Applies to all experiments specified by the aggregate performance for HadGEM3-GC3.1 N512 ORCA12</t>
   </si>
   <si>
     <t xml:space="preserve">Aggregate (across all realms) performance of &lt;machine name&gt; for model &lt;model name&gt;</t>
@@ -324,7 +324,7 @@
     <t xml:space="preserve">&lt;realm name&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Not applicable, applies to all experiments specified by the aggregate performance for &lt;model name&gt;</t>
+    <t xml:space="preserve">Applies to all experiments specified by the aggregate performance for &lt;model name&gt;</t>
   </si>
 </sst>
 </file>
@@ -2674,7 +2674,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>